<commit_message>
Trabajando en estructura para generar rutas (no funcionando)
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -555,7 +555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A0:G9999"/>
+  <dimension ref="A0:H9999"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
@@ -598,74 +598,124 @@
     <row r="1" ht="15" customHeight="1" s="5">
       <c r="A1" s="4" t="inlineStr">
         <is>
-          <t>16742249-7</t>
+          <t>ESTADO</t>
         </is>
       </c>
       <c r="B1" s="4" t="inlineStr">
         <is>
-          <t>Isaias Andres Beroiza Mora</t>
+          <t>RUT</t>
         </is>
       </c>
       <c r="C1" s="4" t="inlineStr">
         <is>
-          <t>colaco sn km3 parcela9</t>
+          <t>CLIENTE</t>
         </is>
       </c>
       <c r="D1" s="4" t="inlineStr">
         <is>
-          <t>calbuco</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="E1" s="4" t="inlineStr">
         <is>
-          <t>988809704</t>
+          <t>COMUNA</t>
         </is>
       </c>
       <c r="F1" s="4" t="inlineStr">
         <is>
-          <t>buscando coordenadas</t>
+          <t>TELEFONO</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr"/>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>GPS</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>OTRO</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>16.742.249-7</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>Isaias Beroiza Mora</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>colaco sn km3 parcela 9</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="4" t="inlineStr">
         <is>
           <t>Calbuco</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="4" t="inlineStr">
         <is>
           <t>56988809704</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>por buscar</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
       </c>
     </row>
-    <row r="3"/>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>activo</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Isaias Andres Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>56988809704</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>buscando coordenadas</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Cliente prueba</t>
+        </is>
+      </c>
+    </row>
     <row r="4"/>
     <row r="5"/>
     <row r="6"/>

</xml_diff>

<commit_message>
Implementado user session system
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -550,7 +550,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -601,13 +601,42 @@
       </c>
     </row>
     <row r="2" ht="13.5" customHeight="1" s="5">
-      <c r="A2" s="4" t="n"/>
-      <c r="B2" s="4" t="n"/>
-      <c r="C2" s="4" t="n"/>
-      <c r="D2" s="4" t="n"/>
-      <c r="E2" s="4" t="n"/>
-      <c r="F2" s="4" t="n"/>
-      <c r="G2" s="4" t="n"/>
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>activo</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>17234876-8</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>Sigo</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>Kosovo</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>Cloac</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>88873234</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="5"/>
   </sheetData>
@@ -623,7 +652,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
@@ -700,13 +729,12 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>20240701</t>
         </is>
       </c>
     </row>
-    <row r="4"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Refactorizando codigo para op
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -2,7 +2,6 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -15,46 +14,32 @@
     <sheet name="gastos_bd" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="0"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
-      <family val="2"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
-      <family val="0"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -79,53 +64,34 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
-    <cellStyle name="Normal 2" xfId="6"/>
+  <cellStyles count="1">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -415,7 +381,7 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
@@ -483,57 +449,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
   <cols>
-    <col width="10.14" customWidth="1" style="4" min="1" max="1"/>
-    <col width="11.57" customWidth="1" style="4" min="2" max="2"/>
-    <col width="40.43" customWidth="1" style="4" min="3" max="3"/>
+    <col width="10.136719" customWidth="1" style="1" min="1" max="1"/>
+    <col width="11.566406" customWidth="1" style="1" min="2" max="2"/>
+    <col width="40.429688" customWidth="1" style="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" s="5">
-      <c r="A1" s="6" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="4">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>usuario</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>contrasena</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>token</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="5">
-      <c r="A2" s="4" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="4">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>iberoiza</t>
         </is>
       </c>
-      <c r="B2" s="4" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>m5m5jaibhcm5gddgk7</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentOddEven="0" differentFirst="0">
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>
@@ -546,377 +510,365 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="5">
-      <c r="A1" s="7" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>ESTADO</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>RUT</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>CLIENTE</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>DIRECCION</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>COMUNA</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>TELEFONO</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>GPS</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>OTRO</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="13.5" customHeight="1" s="5">
-      <c r="A2" s="4" t="inlineStr">
+    <row r="2" ht="13.5" customHeight="1" s="4">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>activo</t>
         </is>
       </c>
-      <c r="B2" s="4" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>17234876-8</t>
         </is>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>Sigo</t>
         </is>
       </c>
-      <c r="D2" s="4" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>Kosovo</t>
         </is>
       </c>
-      <c r="E2" s="4" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>Cloac</t>
         </is>
       </c>
-      <c r="F2" s="4" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>88873234</t>
         </is>
       </c>
-      <c r="G2" s="4" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="0" t="inlineStr">
         <is>
           <t>Test</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="13.5" customHeight="1" s="5"/>
+    <row r="3" ht="13.5" customHeight="1" s="4"/>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1"/>
   <cols>
-    <col width="13.45" customWidth="1" style="4" min="1" max="1"/>
-    <col width="16.31" customWidth="1" style="4" min="7" max="7"/>
-    <col width="15.32" customWidth="1" style="4" min="8" max="8"/>
-    <col width="23.91" customWidth="1" style="4" min="9" max="9"/>
+    <col width="13.449219" customWidth="1" style="1" min="1" max="1"/>
+    <col width="16.308594" customWidth="1" style="1" min="7" max="7"/>
+    <col width="15.316406" customWidth="1" style="1" min="8" max="8"/>
+    <col width="23.90625" customWidth="1" style="1" min="9" max="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="5">
-      <c r="A1" s="6" t="inlineStr">
+    <row r="1" ht="12.8" customHeight="1" s="4">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Ruta actual: </t>
         </is>
       </c>
-      <c r="B1" s="6" t="n"/>
-      <c r="C1" s="6" t="n"/>
-      <c r="D1" s="6" t="n"/>
-      <c r="E1" s="6" t="n"/>
-      <c r="F1" s="6" t="n"/>
-      <c r="G1" s="6" t="n"/>
-      <c r="H1" s="7" t="n"/>
-      <c r="I1" s="7" t="n"/>
-    </row>
-    <row r="2" ht="15" customHeight="1" s="5">
-      <c r="A2" s="6" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>20240706</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="3" t="n"/>
+      <c r="H1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="4">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="B2" s="6" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>RUT</t>
         </is>
       </c>
-      <c r="D2" s="6" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>CLIENTE</t>
         </is>
       </c>
-      <c r="E2" s="6" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>DIRECCION</t>
         </is>
       </c>
-      <c r="F2" s="6" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>COMUNA</t>
         </is>
       </c>
-      <c r="G2" s="6" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>TELEFONO</t>
         </is>
       </c>
-      <c r="H2" s="7" t="inlineStr">
+      <c r="H2" s="3" t="inlineStr">
         <is>
           <t>COORDENADAS</t>
         </is>
       </c>
-      <c r="I2" s="7" t="inlineStr">
+      <c r="I2" s="3" t="inlineStr">
         <is>
           <t>OTRO</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="4" t="inlineStr">
-        <is>
-          <t>20240701</t>
-        </is>
-      </c>
-    </row>
+    <row r="3" ht="15" customHeight="1" s="4"/>
+    <row r="4" ht="15" customHeight="1" s="4"/>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="5">
-      <c r="A1" s="6" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="4">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>RUT</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>CLIENTE</t>
         </is>
       </c>
-      <c r="E1" s="6" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>DIRECCION</t>
         </is>
       </c>
-      <c r="F1" s="6" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>COMUNA</t>
         </is>
       </c>
-      <c r="G1" s="6" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>TELEFONO</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>COORDENADAS</t>
         </is>
       </c>
-      <c r="I1" s="7" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>OTRO</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.54296875" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="13.5" zeroHeight="1"/>
   <cols>
-    <col width="12.68" customWidth="1" style="4" min="2" max="2"/>
-    <col width="13.45" customWidth="1" style="4" min="4" max="4"/>
-    <col width="12.13" customWidth="1" style="4" min="5" max="5"/>
-    <col width="9.140000000000001" customWidth="1" style="4" min="1020" max="1024"/>
+    <col width="12.6796875" customWidth="1" style="1" min="2" max="2"/>
+    <col width="13.449219" customWidth="1" style="1" min="4" max="4"/>
+    <col width="12.128906" customWidth="1" style="1" min="5" max="5"/>
+    <col width="9.136718999999999" customWidth="1" style="1" min="1020" max="1024"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="5">
-      <c r="A1" s="6" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="4">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>RUTA</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>C.REALIZADAS</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>C.NO REALIZADAS</t>
         </is>
       </c>
-      <c r="E1" s="6" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>C.CERRADAS</t>
         </is>
       </c>
-      <c r="F1" s="6" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>OTROS</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="13.5" customHeight="1" s="5">
-      <c r="A2" s="4" t="n"/>
-    </row>
-    <row r="3" ht="13.5" customHeight="1" s="5">
-      <c r="A3" s="4" t="n"/>
-    </row>
-    <row r="4" ht="13.5" customHeight="1" s="5">
-      <c r="A4" s="4" t="n"/>
+    <row r="2" ht="13.5" customHeight="1" s="4">
+      <c r="A2" s="1" t="n"/>
+    </row>
+    <row r="3" ht="13.5" customHeight="1" s="4">
+      <c r="A3" s="1" t="n"/>
+    </row>
+    <row r="4" ht="13.5" customHeight="1" s="4">
+      <c r="A4" s="1" t="n"/>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.1640625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75" zeroHeight="1"/>
   <cols>
-    <col width="27.78" customWidth="1" style="4" min="3" max="3"/>
+    <col width="27.777344" customWidth="1" style="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customHeight="1" s="5">
-      <c r="A1" s="7" t="inlineStr">
+    <row r="1" ht="13.5" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>MONTO</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>DESCRIPCION</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentOddEven="0" differentFirst="0">
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>

</xml_diff>

<commit_message>
Refactorizando codigo y trabajando en funciones
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -75,7 +75,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -86,6 +86,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -466,7 +469,7 @@
     <col width="40.429688" customWidth="1" style="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="4">
+    <row r="1" ht="15" customHeight="1" s="5">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>usuario</t>
@@ -483,7 +486,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="4">
+    <row r="2" ht="15" customHeight="1" s="5">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>iberoiza</t>
@@ -514,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,7 +525,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="4">
+    <row r="1" ht="15" customHeight="1" s="5">
       <c r="A1" s="3" t="inlineStr">
         <is>
           <t>ESTADO</t>
@@ -564,7 +567,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="13.5" customHeight="1" s="4">
+    <row r="2" ht="13.5" customHeight="1" s="5">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>activo</t>
@@ -602,7 +605,49 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="13.5" customHeight="1" s="4"/>
+    <row r="3" ht="13.5" customHeight="1" s="5">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>activo</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>16742249-7</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Isaías Beroiza mora</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Colacao sin</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>988809704</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Por buscar</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+    </row>
+    <row r="4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
 </worksheet>
@@ -617,7 +662,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1"/>
@@ -628,7 +673,7 @@
     <col width="23.90625" customWidth="1" style="1" min="9" max="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="4">
+    <row r="1" ht="12.8" customHeight="1" s="5">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Ruta actual: </t>
@@ -636,7 +681,7 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>20240706</t>
+          <t>20240707</t>
         </is>
       </c>
       <c r="C1" s="2" t="n"/>
@@ -646,7 +691,7 @@
       <c r="G1" s="3" t="n"/>
       <c r="H1" s="3" t="n"/>
     </row>
-    <row r="2" ht="15" customHeight="1" s="4">
+    <row r="2" ht="15" customHeight="1" s="5">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>FECHA</t>
@@ -693,8 +738,44 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="4"/>
-    <row r="4" ht="15" customHeight="1" s="4"/>
+    <row r="3" ht="15" customHeight="1" s="5">
+      <c r="A3" s="1" t="n">
+        <v>20240707</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>167422497</v>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>IABM</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>Colaco sn</t>
+        </is>
+      </c>
+      <c r="F3" s="0" t="inlineStr">
+        <is>
+          <t>calbuco</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>88866455</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>8.654445667754336e+17</v>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>cliente test</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="5"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
 </worksheet>
@@ -714,7 +795,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="4">
+    <row r="1" ht="15" customHeight="1" s="5">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>FECHA</t>
@@ -786,7 +867,7 @@
     <col width="9.136718999999999" customWidth="1" style="1" min="1020" max="1024"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="4">
+    <row r="1" ht="15" customHeight="1" s="5">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>FECHA</t>
@@ -818,13 +899,13 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="13.5" customHeight="1" s="4">
+    <row r="2" ht="13.5" customHeight="1" s="5">
       <c r="A2" s="1" t="n"/>
     </row>
-    <row r="3" ht="13.5" customHeight="1" s="4">
+    <row r="3" ht="13.5" customHeight="1" s="5">
       <c r="A3" s="1" t="n"/>
     </row>
-    <row r="4" ht="13.5" customHeight="1" s="4">
+    <row r="4" ht="13.5" customHeight="1" s="5">
       <c r="A4" s="1" t="n"/>
     </row>
   </sheetData>
@@ -849,7 +930,7 @@
     <col width="27.777344" customWidth="1" style="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customHeight="1" s="4">
+    <row r="1" ht="13.5" customHeight="1" s="5">
       <c r="A1" s="3" t="inlineStr">
         <is>
           <t>FECHA</t>

</xml_diff>

<commit_message>
refactorizando: Trabajando en clientes a ruta
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,48 +606,131 @@
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="5">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="0" t="inlineStr">
         <is>
           <t>activo</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>16742249-7</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>Isaías Beroiza mora</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>Colacao sin</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="0" t="inlineStr">
         <is>
           <t>Calbuco</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="0" t="inlineStr">
         <is>
           <t>988809704</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="0" t="inlineStr">
         <is>
           <t>Por buscar</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" s="0" t="inlineStr">
         <is>
           <t>Test</t>
         </is>
       </c>
     </row>
-    <row r="4"/>
+    <row r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>activo</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="H4" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>activo</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>17673326-8</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>Maria Jose Rodriguez</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>88809704</t>
+        </is>
+      </c>
+      <c r="G5" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="H5" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
 </worksheet>
@@ -659,7 +742,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
@@ -775,7 +858,97 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" s="5"/>
+    <row r="4" ht="15" customHeight="1" s="5">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>20240707</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H4" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>20240707</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>17673326-8</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Maria Jose Rodriguez</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>88809704</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="6"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
 </worksheet>

</xml_diff>

<commit_message>
trabajando en logica confirma cliente ruta
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -742,7 +742,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
@@ -821,134 +821,8 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="5">
-      <c r="A3" s="1" t="n">
-        <v>20240707</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>167422497</v>
-      </c>
-      <c r="D3" s="0" t="inlineStr">
-        <is>
-          <t>IABM</t>
-        </is>
-      </c>
-      <c r="E3" s="0" t="inlineStr">
-        <is>
-          <t>Colaco sn</t>
-        </is>
-      </c>
-      <c r="F3" s="0" t="inlineStr">
-        <is>
-          <t>calbuco</t>
-        </is>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>88866455</v>
-      </c>
-      <c r="H3" s="4" t="n">
-        <v>8.654445667754336e+17</v>
-      </c>
-      <c r="I3" s="1" t="inlineStr">
-        <is>
-          <t>cliente test</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1" s="5">
-      <c r="A4" s="0" t="inlineStr">
-        <is>
-          <t>20240707</t>
-        </is>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>16.742.249-7</t>
-        </is>
-      </c>
-      <c r="D4" s="0" t="inlineStr">
-        <is>
-          <t>Isaias Beroiza Mora</t>
-        </is>
-      </c>
-      <c r="E4" s="0" t="inlineStr">
-        <is>
-          <t>colaco sn km3 parcela 9</t>
-        </is>
-      </c>
-      <c r="F4" s="0" t="inlineStr">
-        <is>
-          <t>Calbuco</t>
-        </is>
-      </c>
-      <c r="G4" s="0" t="inlineStr">
-        <is>
-          <t>88809703</t>
-        </is>
-      </c>
-      <c r="H4" s="0" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="I4" s="0" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>20240707</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>17673326-8</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Maria Jose Rodriguez</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>colaco sn km3 parcela 9</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>ca</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>88809704</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="6"/>
+    <row r="3" ht="15" customHeight="1" s="5"/>
+    <row r="4" ht="15" customHeight="1" s="5"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
 </worksheet>

</xml_diff>

<commit_message>
Trabajando en logica de rutas
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -977,14 +977,23 @@
           <t>20240710</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Test</t>
         </is>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="4">
-      <c r="A3" s="3" t="n"/>
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>20240810</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="4">
       <c r="A4" s="3" t="n"/>

</xml_diff>

<commit_message>
Trabajand en logica de rutas
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -925,7 +925,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -989,15 +989,49 @@
           <t>20240810</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Test</t>
         </is>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="4">
-      <c r="A4" s="3" t="n"/>
-    </row>
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>20240713</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>ruta ejemplo</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>20240714</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>ruta ejemplo</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>20240702</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ruta ejemplo</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
trabajando en logica ruta, bug desconocido
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -1032,12 +1032,12 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>20240720</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>ruta de test</t>
         </is>

</xml_diff>

<commit_message>
trabajando en registro de rutas
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -478,7 +478,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1" outlineLevelRow="0"/>
   <cols>
     <col width="10.14" customWidth="1" style="3" min="1" max="1"/>
     <col width="11.57" customWidth="1" style="3" min="2" max="2"/>
@@ -768,7 +768,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1" outlineLevelRow="0"/>
   <cols>
     <col width="13.45" customWidth="1" style="3" min="1" max="1"/>
     <col width="16.31" customWidth="1" style="3" min="7" max="7"/>
@@ -784,12 +784,12 @@
       </c>
       <c r="B1" s="5" t="inlineStr">
         <is>
-          <t>20240726</t>
+          <t>20240722</t>
         </is>
       </c>
       <c r="C1" s="5" t="inlineStr">
         <is>
-          <t>ruta ejemplo</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="D1" s="5" t="inlineStr"/>
@@ -860,7 +860,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
@@ -917,6 +917,56 @@
       <c r="J1" s="5" t="inlineStr">
         <is>
           <t>SITUACION</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>20240726</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
         </is>
       </c>
     </row>
@@ -939,7 +989,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="13.5" zeroHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="13.5" zeroHeight="1" outlineLevelRow="0"/>
   <cols>
     <col width="12.68" customWidth="1" style="3" min="2" max="2"/>
     <col width="13.45" customWidth="1" style="3" min="4" max="4"/>
@@ -1043,17 +1093,45 @@
           <t>20240726</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>ruta ejemplo</t>
         </is>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="4">
-      <c r="A7" s="3" t="n"/>
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>20240726</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>ruta ejemplo</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>RUTA FINALIZADA</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="4">
-      <c r="A8" s="3" t="n"/>
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>20240722</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="4">
       <c r="A9" s="3" t="n"/>
@@ -1102,7 +1180,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75" zeroHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75" zeroHeight="1" outlineLevelRow="0"/>
   <cols>
     <col width="27.78" customWidth="1" style="3" min="3" max="3"/>
   </cols>

</xml_diff>

<commit_message>
Trabajando en logica de rutas, casi completa
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="usuarios" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,39 +14,26 @@
     <sheet name="gastos_bd" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="0"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
-      <family val="0"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -72,45 +58,31 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -400,7 +372,7 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
@@ -468,57 +440,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
   <cols>
-    <col width="10.14" customWidth="1" style="3" min="1" max="1"/>
-    <col width="11.57" customWidth="1" style="3" min="2" max="2"/>
-    <col width="40.43" customWidth="1" style="3" min="3" max="3"/>
+    <col width="10.136719" customWidth="1" style="1" min="1" max="1"/>
+    <col width="11.566406" customWidth="1" style="1" min="2" max="2"/>
+    <col width="40.429688" customWidth="1" style="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="4">
-      <c r="A1" s="5" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="3">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>usuario</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>contrasena</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>token</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="4">
-      <c r="A2" s="3" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="3">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>iberoiza</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>m5m5jaibhcm5gddgk7</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentOddEven="0" differentFirst="0">
+  <pageSetup paperSize="9"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>
@@ -531,829 +502,1068 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="4">
-      <c r="A1" s="5" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="3">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>ESTADO</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>RUT</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>CLIENTE</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>DIRECCION</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>COMUNA</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>TELEFONO</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>GPS</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>OTRO</t>
         </is>
       </c>
-    </row>
-    <row r="2" ht="13.5" customHeight="1" s="4">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="I1" s="0" t="inlineStr">
+        <is>
+          <t>ULTIMO RETIRO</t>
+        </is>
+      </c>
+      <c r="J1" s="0" t="inlineStr">
+        <is>
+          <t>DIAS CONTRATADOS</t>
+        </is>
+      </c>
+      <c r="K1" s="0" t="inlineStr">
+        <is>
+          <t>PROXIMO RETIRO</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="13.5" customHeight="1" s="3">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>activo</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>17234876-8</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>Sigo</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>Kosovo</t>
         </is>
       </c>
-      <c r="E2" s="3" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>Cloac</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>88873234</t>
         </is>
       </c>
-      <c r="G2" s="3" t="n"/>
-      <c r="H2" s="3" t="inlineStr">
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>Test</t>
         </is>
       </c>
-    </row>
-    <row r="3" ht="13.5" customHeight="1" s="4">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="I2" s="0" t="inlineStr">
+        <is>
+          <t>20240801</t>
+        </is>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="K2" s="0" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="3">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>activo</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>16742249-7</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>Isaías Beroiza mora</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>Colacao sin</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
         <is>
           <t>Calbuco</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>988809704</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>Por buscar</t>
-        </is>
-      </c>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1" s="4">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="I3" s="0" t="inlineStr">
+        <is>
+          <t>20240802</t>
+        </is>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="K3" s="0" t="inlineStr">
+        <is>
+          <t>2024-12-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="3">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>activo</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>16.742.249-7</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>Isaias Beroiza Mora</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>17673326-8</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>Maria Jose Rodriguez</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
         <is>
           <t>colaco sn km3 parcela 9</t>
         </is>
       </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>Calbuco</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>88809703</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="inlineStr">
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>88809704</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
         <is>
           <t>por buscar</t>
         </is>
       </c>
-      <c r="H4" s="3" t="inlineStr">
+      <c r="H4" s="1" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
       </c>
-    </row>
-    <row r="5" ht="15" customHeight="1" s="4">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>activo</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>17673326-8</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>Maria Jose Rodriguez</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>colaco sn km3 parcela 9</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>ca</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>88809704</t>
-        </is>
-      </c>
-      <c r="G5" s="3" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="H5" s="3" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t>20240801</t>
+        </is>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="K4" s="0" t="inlineStr">
+        <is>
+          <t>2024-08-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" hidden="1" ht="15" customHeight="1" s="3"/>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1"/>
   <cols>
-    <col width="13.45" customWidth="1" style="3" min="1" max="1"/>
-    <col width="16.31" customWidth="1" style="3" min="7" max="7"/>
-    <col width="15.32" customWidth="1" style="3" min="8" max="8"/>
-    <col width="23.91" customWidth="1" style="3" min="9" max="9"/>
+    <col width="13.449219" customWidth="1" style="1" min="1" max="1"/>
+    <col width="16.308594" customWidth="1" style="1" min="7" max="7"/>
+    <col width="15.316406" customWidth="1" style="1" min="8" max="8"/>
+    <col width="23.90625" customWidth="1" style="1" min="9" max="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" s="4">
-      <c r="A1" s="5" t="inlineStr">
+    <row r="1" s="3">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Ruta actual: </t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr"/>
-      <c r="C1" s="5" t="inlineStr"/>
-      <c r="D1" s="5" t="inlineStr"/>
-      <c r="E1" s="5" t="inlineStr"/>
-      <c r="F1" s="5" t="inlineStr"/>
-      <c r="G1" s="5" t="n"/>
-      <c r="H1" s="5" t="n"/>
-    </row>
-    <row r="2" ht="15" customHeight="1" s="4">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr"/>
+      <c r="C1" s="2" t="inlineStr"/>
+      <c r="D1" s="2" t="inlineStr"/>
+      <c r="E1" s="2" t="inlineStr"/>
+      <c r="F1" s="2" t="inlineStr"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="3">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>RUT</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>CLIENTE</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>DIRECCION</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>COMUNA</t>
         </is>
       </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>TELEFONO</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="H2" s="2" t="inlineStr">
         <is>
           <t>COORDENADAS</t>
         </is>
       </c>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>OTRO</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="4"/>
-    <row r="4" ht="15" customHeight="1" s="4"/>
+    <row r="3" ht="15" customHeight="1" s="3"/>
+    <row r="4" ht="15" customHeight="1" s="3"/>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="36" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="36" zeroHeight="1"/>
   <sheetData>
-    <row r="1" ht="36" customHeight="1" s="4">
-      <c r="A1" s="5" t="inlineStr">
+    <row r="1" ht="36" customHeight="1" s="3">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>RUT</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>CLIENTE</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>DIRECCION</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>COMUNA</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>TELEFONO</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>COORDENADAS</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>OTRO</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>SITUACION</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="14.9" customHeight="1" s="4">
-      <c r="A2" s="3" t="n">
+    <row r="2" ht="14.9" customHeight="1" s="3">
+      <c r="A2" s="1" t="n">
         <v>20240726</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>16.742.249-7</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>Isaias Beroiza Mora</t>
         </is>
       </c>
-      <c r="E2" s="3" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>colaco sn km3 parcela 9</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>Calbuco</t>
         </is>
       </c>
-      <c r="G2" s="3" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>88809703</t>
         </is>
       </c>
-      <c r="H2" s="3" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>por buscar</t>
         </is>
       </c>
-      <c r="I2" s="3" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
       </c>
-      <c r="J2" s="3" t="inlineStr">
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t>REALIZADO</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+    <row r="3" ht="36" customHeight="1" s="3">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>20240701</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>17673326-8</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="D3" s="1" t="inlineStr">
         <is>
           <t>Maria Jose Rodriguez</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="E3" s="1" t="inlineStr">
         <is>
           <t>colaco sn km3 parcela 9</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F3" s="1" t="inlineStr">
         <is>
           <t>ca</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="G3" s="1" t="inlineStr">
         <is>
           <t>88809704</t>
         </is>
       </c>
-      <c r="H3" s="3" t="inlineStr">
+      <c r="H3" s="1" t="inlineStr">
         <is>
           <t>por buscar</t>
         </is>
       </c>
-      <c r="I3" s="3" t="inlineStr">
+      <c r="I3" s="1" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
       </c>
-      <c r="J3" s="3" t="inlineStr">
+      <c r="J3" s="1" t="inlineStr">
         <is>
           <t>REALIZADO</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
+    <row r="4" ht="36" customHeight="1" s="3">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>20240701</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>16.742.249-7</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
+      <c r="D4" s="1" t="inlineStr">
         <is>
           <t>Isaias Beroiza Mora</t>
         </is>
       </c>
-      <c r="E4" s="3" t="inlineStr">
+      <c r="E4" s="1" t="inlineStr">
         <is>
           <t>colaco sn km3 parcela 9</t>
         </is>
       </c>
-      <c r="F4" s="3" t="inlineStr">
+      <c r="F4" s="1" t="inlineStr">
         <is>
           <t>Calbuco</t>
         </is>
       </c>
-      <c r="G4" s="3" t="inlineStr">
+      <c r="G4" s="1" t="inlineStr">
         <is>
           <t>88809703</t>
         </is>
       </c>
-      <c r="H4" s="3" t="inlineStr">
+      <c r="H4" s="1" t="inlineStr">
         <is>
           <t>por buscar</t>
         </is>
       </c>
-      <c r="I4" s="3" t="inlineStr">
+      <c r="I4" s="1" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
       </c>
-      <c r="J4" s="3" t="inlineStr">
+      <c r="J4" s="1" t="inlineStr">
         <is>
           <t>POSPUESTO</t>
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>20240801</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>17234876-8</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>Sigo</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>Kosovo</t>
+        </is>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>Cloac</t>
+        </is>
+      </c>
+      <c r="G5" s="0" t="inlineStr">
+        <is>
+          <t>88873234</t>
+        </is>
+      </c>
+      <c r="I5" s="0" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="J5" s="0" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>20240801</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G6" s="0" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H6" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I6" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J6" s="0" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>20240801</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>17673326-8</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>Maria Jose Rodriguez</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="G7" s="0" t="inlineStr">
+        <is>
+          <t>88809704</t>
+        </is>
+      </c>
+      <c r="H7" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I7" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J7" s="0" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>20240802</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G8" s="0" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H8" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I8" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J8" s="0" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="13.5" zeroHeight="1" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="13.5" zeroHeight="1"/>
   <cols>
-    <col width="12.68" customWidth="1" style="3" min="2" max="2"/>
-    <col width="13.45" customWidth="1" style="3" min="4" max="4"/>
-    <col width="12.13" customWidth="1" style="3" min="5" max="5"/>
-    <col width="9.140000000000001" customWidth="1" style="3" min="1020" max="1024"/>
+    <col width="12.6796875" customWidth="1" style="1" min="2" max="2"/>
+    <col width="13.449219" customWidth="1" style="1" min="4" max="4"/>
+    <col width="12.128906" customWidth="1" style="1" min="5" max="5"/>
+    <col width="9.136718999999999" customWidth="1" style="1" min="1020" max="1024"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="4">
-      <c r="A1" s="5" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="3">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>RUTA</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>C.REALIZADAS</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>C.NO REALIZADAS</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>C.CERRADAS</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>OTROS</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="13.5" customHeight="1" s="4">
-      <c r="A2" s="3" t="inlineStr">
+    <row r="2" ht="13.5" customHeight="1" s="3">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>20240721</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>ruta ejemplo</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="13.5" customHeight="1" s="4">
-      <c r="A3" s="3" t="inlineStr">
+    <row r="3" ht="13.5" customHeight="1" s="3">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>20240721</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>ruta ejemplo</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F3" s="1" t="inlineStr">
         <is>
           <t>RUTA FINALIZADA</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="13.5" customHeight="1" s="4">
-      <c r="A4" s="3" t="inlineStr">
+    <row r="4" ht="13.5" customHeight="1" s="3">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>20240721</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>ruta ejemplo</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="13.5" customHeight="1" s="4">
-      <c r="A5" s="3" t="inlineStr">
+    <row r="5" ht="13.5" customHeight="1" s="3">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>20240721</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>ruta ejemplo</t>
         </is>
       </c>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="F5" s="1" t="inlineStr">
         <is>
           <t>RUTA FINALIZADA</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="13.5" customHeight="1" s="4">
-      <c r="A6" s="3" t="inlineStr">
+    <row r="6" ht="13.5" customHeight="1" s="3">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>20240726</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>ruta ejemplo</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="13.5" customHeight="1" s="4">
-      <c r="A7" s="3" t="inlineStr">
+    <row r="7" ht="13.5" customHeight="1" s="3">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>20240726</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>ruta ejemplo</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="C7" s="1" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="F7" s="1" t="inlineStr">
         <is>
           <t>RUTA FINALIZADA</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="13.5" customHeight="1" s="4">
-      <c r="A8" s="3" t="inlineStr">
+    <row r="8" ht="13.5" customHeight="1" s="3">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>20240722</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" s="1" t="inlineStr">
         <is>
           <t>Test</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="13.5" customHeight="1" s="4">
-      <c r="A9" s="3" t="inlineStr">
+    <row r="9" ht="13.5" customHeight="1" s="3">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>20240722</t>
         </is>
       </c>
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B9" s="1" t="inlineStr">
         <is>
           <t>Test</t>
         </is>
       </c>
-      <c r="F9" s="3" t="inlineStr">
+      <c r="F9" s="1" t="inlineStr">
         <is>
           <t>RUTA FINALIZADA</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="13.5" customHeight="1" s="4">
-      <c r="A10" s="3" t="inlineStr">
+    <row r="10" ht="13.5" customHeight="1" s="3">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>20240726</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" s="1" t="inlineStr">
         <is>
           <t>ruta de prueba</t>
         </is>
       </c>
-      <c r="F10" s="3" t="inlineStr">
+      <c r="F10" s="1" t="inlineStr">
         <is>
           <t>RUTA FINALIZADA</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="13.5" customHeight="1" s="4">
-      <c r="A11" s="3" t="inlineStr">
+    <row r="11" ht="13.5" customHeight="1" s="3">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>20240701</t>
         </is>
       </c>
-      <c r="B11" s="3" t="inlineStr">
+      <c r="B11" s="1" t="inlineStr">
         <is>
           <t>ruta TEST</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="13.5" customHeight="1" s="4">
-      <c r="A12" s="3" t="inlineStr">
+    <row r="12" ht="13.5" customHeight="1" s="3">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>20240701</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr">
         <is>
           <t>ruta TEST</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" s="0" t="inlineStr">
         <is>
           <t>RUTA FINALIZADA</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="13.5" customHeight="1" s="4">
-      <c r="A13" s="3" t="n"/>
-    </row>
-    <row r="14" ht="13.5" customHeight="1" s="4">
-      <c r="A14" s="3" t="n"/>
-    </row>
-    <row r="15" ht="13.5" customHeight="1" s="4">
-      <c r="A15" s="3" t="n"/>
-    </row>
-    <row r="16" ht="13.5" customHeight="1" s="4">
-      <c r="A16" s="3" t="n"/>
-    </row>
-    <row r="17" ht="13.5" customHeight="1" s="4">
-      <c r="A17" s="3" t="n"/>
-    </row>
-    <row r="18" ht="13.5" customHeight="1" s="4"/>
+    <row r="13" ht="13.5" customHeight="1" s="3">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>20240801</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>Ruta Test</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F13" s="0" t="inlineStr">
+        <is>
+          <t>RUTA FINALIZADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="13.5" customHeight="1" s="3">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>20240802</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>ruta TEST</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>RUTA FINALIZADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="13.5" customHeight="1" s="3">
+      <c r="A15" s="1" t="n"/>
+    </row>
+    <row r="16" ht="13.5" customHeight="1" s="3">
+      <c r="A16" s="1" t="n"/>
+    </row>
+    <row r="17" ht="13.5" customHeight="1" s="3">
+      <c r="A17" s="1" t="n"/>
+    </row>
+    <row r="18" ht="13.5" customHeight="1" s="3"/>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75" zeroHeight="1" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75" zeroHeight="1"/>
   <cols>
-    <col width="27.78" customWidth="1" style="3" min="3" max="3"/>
+    <col width="27.777344" customWidth="1" style="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customHeight="1" s="4">
-      <c r="A1" s="5" t="inlineStr">
+    <row r="1" ht="13.5" customHeight="1" s="3">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>MONTO</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>DESCRIPCION</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentOddEven="0" differentFirst="0">
+  <pageSetup paperSize="9"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>

</xml_diff>

<commit_message>
Trabajando en logica confpos
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -665,7 +665,7 @@
       </c>
       <c r="I3" s="0" t="inlineStr">
         <is>
-          <t>20240802</t>
+          <t>20240831</t>
         </is>
       </c>
       <c r="J3" s="0" t="n">
@@ -673,7 +673,7 @@
       </c>
       <c r="K3" s="0" t="inlineStr">
         <is>
-          <t>2024-12-02</t>
+          <t>2024-12-31</t>
         </is>
       </c>
     </row>
@@ -834,7 +834,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -1234,6 +1234,61 @@
       <c r="J8" s="0" t="inlineStr">
         <is>
           <t>REALIZADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>20240831</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E9" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G9" s="0" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H9" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I9" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J9" s="0" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+      <c r="K9" s="0" t="inlineStr">
+        <is>
+          <t>3c3l1ba ok</t>
         </is>
       </c>
     </row>
@@ -1501,17 +1556,36 @@
           <t>ruta TEST</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" s="0" t="inlineStr">
         <is>
           <t>RUTA FINALIZADA</t>
         </is>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" s="3">
-      <c r="A15" s="1" t="n"/>
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>20240831</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>ruta ejemplo</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>RUTA FINALIZADA</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="13.5" customHeight="1" s="3">
       <c r="A16" s="1" t="n"/>

</xml_diff>

<commit_message>
Trabajando en logica de finalizado ruta
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -665,7 +665,7 @@
       </c>
       <c r="I3" s="0" t="inlineStr">
         <is>
-          <t>20240831</t>
+          <t>20240808</t>
         </is>
       </c>
       <c r="J3" s="0" t="n">
@@ -673,7 +673,7 @@
       </c>
       <c r="K3" s="0" t="inlineStr">
         <is>
-          <t>2024-12-31</t>
+          <t>2024-12-08</t>
         </is>
       </c>
     </row>
@@ -834,7 +834,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -1289,6 +1289,171 @@
       <c r="K9" s="0" t="inlineStr">
         <is>
           <t>3c3l1ba ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>20240829</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E10" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F10" s="0" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G10" s="0" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H10" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I10" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J10" s="0" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+      <c r="K10" s="0" t="inlineStr">
+        <is>
+          <t>3c3l1ba ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>20240828</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E11" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F11" s="0" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G11" s="0" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H11" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I11" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J11" s="0" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+      <c r="K11" s="0" t="inlineStr">
+        <is>
+          <t>3c3l1ba ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>20240808</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E12" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G12" s="0" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H12" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I12" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J12" s="0" t="inlineStr">
+        <is>
+          <t>POSPUESTO</t>
+        </is>
+      </c>
+      <c r="K12" s="0" t="inlineStr">
+        <is>
+          <t>DEUDA</t>
         </is>
       </c>
     </row>
@@ -1304,7 +1469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -1576,24 +1741,95 @@
           <t>ruta ejemplo</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" s="0" t="inlineStr">
         <is>
           <t>RUTA FINALIZADA</t>
         </is>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1" s="3">
-      <c r="A16" s="1" t="n"/>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>20240829</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>ruta ejemplo</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
+        <is>
+          <t>RUTA FINALIZADA</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="13.5" customHeight="1" s="3">
-      <c r="A17" s="1" t="n"/>
-    </row>
-    <row r="18" ht="13.5" customHeight="1" s="3"/>
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>20240828</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>ruta test</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>RUTA FINALIZADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="13.5" customHeight="1" s="3">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>20240807</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>ruta test</t>
+        </is>
+      </c>
+      <c r="F18" s="0" t="inlineStr">
+        <is>
+          <t>RUTA FINALIZADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>20240808</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>Ruta ejemplo terminacion</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2024-08-06T15:51:36.376168 RUTA FINALIZADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="20"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9"/>

</xml_diff>

<commit_message>
Corrigiendo parametros y BD
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="usuarios" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,26 +15,39 @@
     <sheet name="gastos_bd" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="0"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="0"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -58,45 +72,67 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="general" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
+      <alignment horizontal="general" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -453,68 +489,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="10.140625" customWidth="1" style="1" min="1" max="1"/>
-    <col width="11.5703125" customWidth="1" style="1" min="2" max="2"/>
-    <col width="40.42578125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="10.14" customWidth="1" style="7" min="1" max="1"/>
+    <col width="11.57" customWidth="1" style="7" min="2" max="2"/>
+    <col width="40.43" customWidth="1" style="7" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="7">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="8">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>usuario</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>contrasena</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>token</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="7">
-      <c r="A2" s="1" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="8">
+      <c r="A2" s="7" t="inlineStr">
         <is>
           <t>iberoiza</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="B2" s="7" t="inlineStr">
         <is>
           <t>m5m5jaibhcm5gddgk7</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+    <row r="3" ht="15" customHeight="1" s="8">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>mauricio</t>
         </is>
       </c>
-      <c r="B3" s="6" t="inlineStr">
+      <c r="B3" s="7" t="inlineStr">
         <is>
           <t>1n9v0w5r@x2o9v$zzm1n$zS&amp;v#5r@x5rYl</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9"/>
-  <headerFooter>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>
@@ -527,732 +564,854 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="10.42578125" customWidth="1" style="7" min="1" max="11"/>
+    <col width="10.43" customWidth="1" style="10" min="1" max="11"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="7">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="8">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>ESTADO</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>RUT</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>CLIENTE</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="9" t="inlineStr">
         <is>
           <t>DIRECCION</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="9" t="inlineStr">
         <is>
           <t>COMUNA</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="9" t="inlineStr">
         <is>
           <t>TELEFONO</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="9" t="inlineStr">
         <is>
           <t>GPS</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="9" t="inlineStr">
         <is>
           <t>OTRO</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="9" t="inlineStr">
         <is>
           <t>ULTIMO RETIRO</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="9" t="inlineStr">
         <is>
           <t>DIAS CONTRATADOS</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="9" t="inlineStr">
         <is>
           <t>PROXIMO RETIRO</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="13.5" customHeight="1" s="7">
-      <c r="A2" s="1" t="inlineStr">
+    <row r="2" ht="13.5" customHeight="1" s="8">
+      <c r="A2" s="7" t="inlineStr">
         <is>
           <t>activo</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="B2" s="7" t="inlineStr">
         <is>
           <t>17234876-8</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
+      <c r="C2" s="7" t="inlineStr">
         <is>
           <t>Sigo</t>
         </is>
       </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="D2" s="7" t="inlineStr">
         <is>
           <t>Kosovo</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="E2" s="7" t="inlineStr">
         <is>
           <t>Cloac</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="F2" s="7" t="inlineStr">
         <is>
           <t>88873234</t>
         </is>
       </c>
-      <c r="G2" s="1" t="n"/>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="G2" s="7" t="n"/>
+      <c r="H2" s="7" t="inlineStr">
         <is>
           <t>Test</t>
         </is>
       </c>
-      <c r="I2" s="6" t="inlineStr">
+      <c r="I2" s="7" t="inlineStr">
         <is>
           <t>20240801</t>
         </is>
       </c>
-      <c r="J2" s="6" t="n">
+      <c r="J2" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="K2" s="6" t="inlineStr">
+      <c r="K2" s="7" t="inlineStr">
         <is>
           <t>2024-09-30</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="7">
-      <c r="A3" s="1" t="inlineStr">
+    <row r="3" ht="15" customHeight="1" s="8">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>activo</t>
         </is>
       </c>
-      <c r="B3" s="1" t="inlineStr">
+      <c r="B3" s="7" t="inlineStr">
         <is>
           <t>16.742.249-7</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
+      <c r="C3" s="7" t="inlineStr">
         <is>
           <t>Isaias Beroiza Mora</t>
         </is>
       </c>
-      <c r="D3" s="1" t="inlineStr">
+      <c r="D3" s="7" t="inlineStr">
         <is>
           <t>colaco sn km3 parcela 9</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
+      <c r="E3" s="7" t="inlineStr">
         <is>
           <t>Calbuco</t>
         </is>
       </c>
-      <c r="F3" s="1" t="inlineStr">
+      <c r="F3" s="7" t="inlineStr">
         <is>
           <t>88809703</t>
         </is>
       </c>
-      <c r="G3" s="1" t="inlineStr">
+      <c r="G3" s="7" t="inlineStr">
         <is>
           <t>por buscar</t>
         </is>
       </c>
-      <c r="H3" s="1" t="inlineStr">
+      <c r="H3" s="7" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
       </c>
-      <c r="I3" s="6" t="inlineStr">
+      <c r="I3" s="7" t="inlineStr">
+        <is>
+          <t>20240813</t>
+        </is>
+      </c>
+      <c r="J3" s="7" t="n">
+        <v>120</v>
+      </c>
+      <c r="K3" s="7" t="inlineStr">
+        <is>
+          <t>2024-12-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="8">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>activo</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>17673326-8</t>
+        </is>
+      </c>
+      <c r="C4" s="7" t="inlineStr">
+        <is>
+          <t>Maria Jose Rodriguez</t>
+        </is>
+      </c>
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="E4" s="7" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="F4" s="7" t="inlineStr">
+        <is>
+          <t>88809704</t>
+        </is>
+      </c>
+      <c r="G4" s="7" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="I4" s="7" t="inlineStr">
         <is>
           <t>20240801</t>
         </is>
       </c>
-      <c r="J3" s="6" t="n">
-        <v>120</v>
-      </c>
-      <c r="K3" s="6" t="inlineStr">
-        <is>
-          <t>2024-12-01</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1" s="7">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>activo</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>17673326-8</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>Maria Jose Rodriguez</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>colaco sn km3 parcela 9</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>ca</t>
-        </is>
-      </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>88809704</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="I4" s="6" t="inlineStr">
-        <is>
-          <t>20240801</t>
-        </is>
-      </c>
-      <c r="J4" s="6" t="n">
+      <c r="J4" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="K4" s="6" t="inlineStr">
+      <c r="K4" s="7" t="inlineStr">
         <is>
           <t>2024-09-02</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" s="7"/>
+    <row r="5" ht="15" customHeight="1" s="8"/>
   </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="13.42578125" customWidth="1" style="1" min="1" max="1"/>
-    <col width="16.28515625" customWidth="1" style="1" min="7" max="7"/>
-    <col width="15.28515625" customWidth="1" style="1" min="8" max="8"/>
-    <col width="23.85546875" customWidth="1" style="1" min="9" max="9"/>
-    <col width="15.140625" customWidth="1" style="7" min="10" max="10"/>
+    <col width="13.43" customWidth="1" style="7" min="1" max="1"/>
+    <col width="16.28" customWidth="1" style="7" min="7" max="7"/>
+    <col width="15.28" customWidth="1" style="7" min="8" max="8"/>
+    <col width="23.85" customWidth="1" style="7" min="9" max="9"/>
+    <col width="15.14" customWidth="1" style="10" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="8">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Ruta actual: </t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr"/>
-      <c r="C1" s="2" t="inlineStr"/>
-      <c r="D1" s="2" t="inlineStr"/>
-      <c r="E1" s="2" t="inlineStr"/>
-      <c r="F1" s="2" t="n"/>
-      <c r="G1" s="2" t="n"/>
-      <c r="H1" s="2" t="n"/>
-      <c r="I1" s="2" t="n"/>
-      <c r="J1" s="2" t="n"/>
-    </row>
-    <row r="2" ht="15" customHeight="1" s="7">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>20240813</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>Ruta Chiloe-PtoMontt</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9" t="n"/>
+      <c r="F1" s="9" t="n"/>
+      <c r="G1" s="9" t="n"/>
+      <c r="H1" s="9" t="n"/>
+      <c r="I1" s="9" t="n"/>
+      <c r="J1" s="9" t="n"/>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="8">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="9" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="9" t="inlineStr">
         <is>
           <t>RUT</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="9" t="inlineStr">
         <is>
           <t>CLIENTE</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="9" t="inlineStr">
         <is>
           <t>DIRECCION</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="9" t="inlineStr">
         <is>
           <t>COMUNA</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" s="9" t="inlineStr">
         <is>
           <t>TELEFONO</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="H2" s="9" t="inlineStr">
         <is>
           <t>COORDENADAS</t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="I2" s="9" t="inlineStr">
         <is>
           <t>OTRO</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="J2" s="9" t="inlineStr">
         <is>
           <t>ULTIMO RETIRO</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="7"/>
-    <row r="4" ht="15" customHeight="1" s="7"/>
+    <row r="3" ht="15" customHeight="1" s="8">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>20240813</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>17673326-8</t>
+        </is>
+      </c>
+      <c r="D3" s="7" t="inlineStr">
+        <is>
+          <t>Maria Jose Rodriguez</t>
+        </is>
+      </c>
+      <c r="E3" s="7" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F3" s="7" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="G3" s="7" t="inlineStr">
+        <is>
+          <t>88809704</t>
+        </is>
+      </c>
+      <c r="H3" s="7" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I3" s="7" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J3" s="7" t="inlineStr">
+        <is>
+          <t>20240801</t>
+        </is>
+      </c>
+      <c r="K3" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="L3" s="7" t="inlineStr">
+        <is>
+          <t>2024-09-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="8"/>
   </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="10" customWidth="1" style="4" min="1" max="12"/>
+    <col width="10" customWidth="1" style="11" min="1" max="12"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36" customHeight="1" s="7">
-      <c r="A1" s="3" t="inlineStr">
+    <row r="1" ht="36" customHeight="1" s="8">
+      <c r="A1" s="12" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="12" t="inlineStr">
         <is>
           <t>RUT</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
         <is>
           <t>CLIENTE</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>DIRECCION</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="12" t="inlineStr">
         <is>
           <t>COMUNA</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="G1" s="12" t="inlineStr">
         <is>
           <t>TELEFONO</t>
         </is>
       </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="H1" s="12" t="inlineStr">
         <is>
           <t>COORDENADAS</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" s="12" t="inlineStr">
         <is>
           <t>OTRO</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
-        <is>
-          <t>SITUACION</t>
-        </is>
-      </c>
-      <c r="K1" s="3" t="inlineStr">
-        <is>
-          <t>OBSERVACIONES</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="14.85" customHeight="1" s="7">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="J1" s="12" t="inlineStr">
+        <is>
+          <t>ULTIMO RETIRO</t>
+        </is>
+      </c>
+      <c r="K1" s="12" t="inlineStr">
+        <is>
+          <t>STATUS</t>
+        </is>
+      </c>
+      <c r="L1" s="12" t="inlineStr">
+        <is>
+          <t>DETALLES RETIRO</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="14.25" customHeight="1" s="8">
+      <c r="A2" s="11" t="inlineStr">
         <is>
           <t>20240801</t>
         </is>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="11" t="inlineStr">
         <is>
           <t>16.742.249-7</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="D2" s="11" t="inlineStr">
         <is>
           <t>Isaias Beroiza Mora</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="E2" s="11" t="inlineStr">
         <is>
           <t>colaco sn km3 parcela 9</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="11" t="inlineStr">
         <is>
           <t>Calbuco</t>
         </is>
       </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="11" t="inlineStr">
         <is>
           <t>88809703</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="H2" s="11" t="inlineStr">
         <is>
           <t>por buscar</t>
         </is>
       </c>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="I2" s="11" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
       </c>
-      <c r="J2" s="5" t="inlineStr">
+      <c r="J2" s="11" t="inlineStr">
         <is>
           <t>20240808</t>
         </is>
       </c>
-      <c r="K2" s="6" t="inlineStr">
+      <c r="K2" s="7" t="inlineStr">
         <is>
           <t>REALIZADO</t>
         </is>
       </c>
-      <c r="L2" s="6" t="inlineStr">
+      <c r="L2" s="7" t="inlineStr">
         <is>
           <t>1ca3lt</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="36" customHeight="1" s="7">
-      <c r="A3" s="5" t="inlineStr">
+    <row r="3" ht="36" customHeight="1" s="8">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t>20240801</t>
         </is>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="inlineStr">
+      <c r="C3" s="11" t="inlineStr">
         <is>
           <t>17673326-8</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr">
+      <c r="D3" s="11" t="inlineStr">
         <is>
           <t>Maria Jose Rodriguez</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr">
+      <c r="E3" s="11" t="inlineStr">
         <is>
           <t>colaco sn km3 parcela 9</t>
         </is>
       </c>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="F3" s="11" t="inlineStr">
         <is>
           <t>ca</t>
         </is>
       </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="11" t="inlineStr">
         <is>
           <t>88809704</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
+      <c r="H3" s="11" t="inlineStr">
         <is>
           <t>por buscar</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr">
+      <c r="I3" s="11" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
       </c>
-      <c r="J3" s="5" t="inlineStr">
+      <c r="J3" s="11" t="inlineStr">
         <is>
           <t>20240801</t>
         </is>
       </c>
-      <c r="K3" s="6" t="inlineStr">
+      <c r="K3" s="7" t="inlineStr">
         <is>
           <t>REALIZADO</t>
         </is>
       </c>
-      <c r="L3" s="6" t="inlineStr">
+      <c r="L3" s="7" t="inlineStr">
         <is>
           <t>1ca3lt</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="36" customHeight="1" s="7">
-      <c r="A4" s="5" t="n"/>
-      <c r="B4" s="5" t="n"/>
-      <c r="C4" s="5" t="n"/>
-      <c r="D4" s="5" t="n"/>
-      <c r="E4" s="5" t="n"/>
-      <c r="F4" s="5" t="n"/>
-      <c r="G4" s="5" t="n"/>
-      <c r="H4" s="5" t="n"/>
-      <c r="I4" s="5" t="n"/>
-      <c r="J4" s="5" t="n"/>
+    <row r="4" ht="36" customHeight="1" s="8">
+      <c r="A4" s="11" t="inlineStr">
+        <is>
+          <t>20240813</t>
+        </is>
+      </c>
+      <c r="B4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E4" s="11" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F4" s="11" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G4" s="11" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H4" s="11" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I4" s="11" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J4" s="11" t="inlineStr">
+        <is>
+          <t>20240801</t>
+        </is>
+      </c>
+      <c r="K4" s="7" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+      <c r="L4" s="7" t="inlineStr">
+        <is>
+          <t>1ca3lt</t>
+        </is>
+      </c>
     </row>
   </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10" defaultRowHeight="15" zeroHeight="1" outlineLevelRow="0"/>
   <cols>
-    <col width="12.7109375" customWidth="1" style="1" min="2" max="2"/>
-    <col width="13.42578125" customWidth="1" style="1" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="1" min="1019" max="1023"/>
+    <col width="12.71" customWidth="1" style="7" min="2" max="2"/>
+    <col width="13.43" customWidth="1" style="7" min="4" max="4"/>
+    <col width="9.140000000000001" customWidth="1" style="7" min="1019" max="1023"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="7">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="8">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>RUTA</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>C.REALIZADAS</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="9" t="inlineStr">
         <is>
           <t>C.NO REALIZADAS</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="9" t="inlineStr">
         <is>
           <t>OTROS</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="13.5" customHeight="1" s="7">
-      <c r="A2" s="1" t="inlineStr">
+    <row r="2" ht="13.5" customHeight="1" s="8">
+      <c r="A2" s="7" t="inlineStr">
         <is>
           <t>20240801</t>
         </is>
       </c>
-      <c r="B2" s="6" t="inlineStr">
+      <c r="B2" s="7" t="inlineStr">
         <is>
           <t>ruta TEST</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="7" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="7" t="inlineStr">
         <is>
           <t>2024-08-13T18:41:49.495520 RUTA FINALIZADA</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="13.5" customHeight="1" s="7">
-      <c r="A3" s="1" t="n"/>
-      <c r="E3" s="1" t="n"/>
-    </row>
-    <row r="4" ht="13.5" customHeight="1" s="7">
-      <c r="A4" s="1" t="n"/>
-    </row>
-    <row r="5" ht="13.5" customHeight="1" s="7">
-      <c r="A5" s="1" t="n"/>
-      <c r="E5" s="1" t="n"/>
-    </row>
-    <row r="6" ht="13.5" customHeight="1" s="7">
-      <c r="A6" s="1" t="n"/>
-    </row>
-    <row r="7" ht="13.5" customHeight="1" s="7">
-      <c r="A7" s="1" t="n"/>
-      <c r="C7" s="1" t="n"/>
-      <c r="E7" s="1" t="n"/>
-    </row>
-    <row r="8" ht="13.5" customHeight="1" s="7">
-      <c r="A8" s="1" t="n"/>
-    </row>
-    <row r="9" ht="13.5" customHeight="1" s="7">
-      <c r="A9" s="1" t="n"/>
-      <c r="E9" s="1" t="n"/>
-    </row>
-    <row r="10" ht="13.5" customHeight="1" s="7">
-      <c r="A10" s="1" t="n"/>
-      <c r="E10" s="1" t="n"/>
-    </row>
-    <row r="11" ht="13.5" customHeight="1" s="7">
-      <c r="A11" s="1" t="n"/>
-    </row>
-    <row r="12" ht="13.5" customHeight="1" s="7">
-      <c r="A12" s="1" t="n"/>
-      <c r="B12" s="6" t="n"/>
-      <c r="D12" s="6" t="n"/>
-    </row>
-    <row r="13" ht="13.5" customHeight="1" s="7">
-      <c r="A13" s="1" t="n"/>
-      <c r="B13" s="6" t="n"/>
-    </row>
-    <row r="14" ht="13.5" customHeight="1" s="7">
-      <c r="A14" s="1" t="n"/>
-      <c r="B14" s="6" t="n"/>
-    </row>
-    <row r="15" ht="13.5" customHeight="1" s="7">
-      <c r="A15" s="1" t="n"/>
-      <c r="B15" s="6" t="n"/>
-    </row>
-    <row r="16" ht="13.5" customHeight="1" s="7">
-      <c r="A16" s="1" t="n"/>
-      <c r="B16" s="6" t="n"/>
-    </row>
-    <row r="17" ht="13.5" customHeight="1" s="7">
-      <c r="A17" s="1" t="n"/>
-      <c r="B17" s="6" t="n"/>
-    </row>
-    <row r="18" ht="13.5" customHeight="1" s="7">
-      <c r="B18" s="6" t="n"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="6" t="n"/>
-      <c r="D19" s="6" t="n"/>
-    </row>
+    <row r="3" ht="13.5" customHeight="1" s="8">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>20240813</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="inlineStr">
+        <is>
+          <t>Ruta Chiloe-PtoMontt</t>
+        </is>
+      </c>
+      <c r="E3" s="7" t="n"/>
+    </row>
+    <row r="4" ht="13.5" customHeight="1" s="8">
+      <c r="A4" s="7" t="n"/>
+    </row>
+    <row r="5" ht="13.5" customHeight="1" s="8">
+      <c r="A5" s="7" t="n"/>
+      <c r="E5" s="7" t="n"/>
+    </row>
+    <row r="6" ht="13.5" customHeight="1" s="8">
+      <c r="A6" s="7" t="n"/>
+    </row>
+    <row r="7" ht="13.5" customHeight="1" s="8">
+      <c r="A7" s="7" t="n"/>
+      <c r="C7" s="7" t="n"/>
+      <c r="E7" s="7" t="n"/>
+    </row>
+    <row r="8" ht="13.5" customHeight="1" s="8">
+      <c r="A8" s="7" t="n"/>
+    </row>
+    <row r="9" ht="13.5" customHeight="1" s="8">
+      <c r="A9" s="7" t="n"/>
+      <c r="E9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="13.5" customHeight="1" s="8">
+      <c r="A10" s="7" t="n"/>
+      <c r="E10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="13.5" customHeight="1" s="8">
+      <c r="A11" s="7" t="n"/>
+    </row>
+    <row r="12" ht="13.5" customHeight="1" s="8">
+      <c r="A12" s="7" t="n"/>
+    </row>
+    <row r="13" ht="13.5" customHeight="1" s="8">
+      <c r="A13" s="7" t="n"/>
+    </row>
+    <row r="14" ht="13.5" customHeight="1" s="8">
+      <c r="A14" s="7" t="n"/>
+    </row>
+    <row r="15" ht="13.5" customHeight="1" s="8">
+      <c r="A15" s="7" t="n"/>
+    </row>
+    <row r="16" ht="13.5" customHeight="1" s="8">
+      <c r="A16" s="7" t="n"/>
+    </row>
+    <row r="17" ht="13.5" customHeight="1" s="8">
+      <c r="A17" s="7" t="n"/>
+    </row>
+    <row r="18" ht="13.5" customHeight="1" s="8"/>
+    <row r="19" ht="15" customHeight="1" s="8"/>
   </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="27.7109375" customWidth="1" style="1" min="3" max="3"/>
+    <col width="27.72" customWidth="1" style="7" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customHeight="1" s="7">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="13.5" customHeight="1" s="8">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>MONTO</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>DESCRIPCION</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9"/>
-  <headerFooter>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>

</xml_diff>

<commit_message>
Refactorizaciones finales y pruebas
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -785,7 +785,7 @@
       </c>
       <c r="I4" s="7" t="inlineStr">
         <is>
-          <t>20240801</t>
+          <t>2024-08-13</t>
         </is>
       </c>
       <c r="J4" s="7" t="n">
@@ -793,11 +793,57 @@
       </c>
       <c r="K4" s="7" t="inlineStr">
         <is>
-          <t>2024-09-02</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1" s="8"/>
+          <t>2024-09-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" s="8">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>activo</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>15437239-7</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>Ishovias</t>
+        </is>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>cloacsoin sn</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="inlineStr">
+        <is>
+          <t>Salhued</t>
+        </is>
+      </c>
+      <c r="F5" s="7" t="inlineStr">
+        <is>
+          <t>99953274</t>
+        </is>
+      </c>
+      <c r="G5" s="7" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>Cliente test</t>
+        </is>
+      </c>
+      <c r="I5" s="7" t="inlineStr">
+        <is>
+          <t>2024-08-22</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -811,7 +857,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -832,20 +878,10 @@
           <t xml:space="preserve">Ruta actual: </t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
-        <is>
-          <t>20240813</t>
-        </is>
-      </c>
-      <c r="C1" s="9" t="inlineStr">
-        <is>
-          <t>Ruta Chiloe-PtoMontt</t>
-        </is>
-      </c>
-      <c r="D1" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E1" s="9" t="n"/>
+      <c r="B1" s="9" t="inlineStr"/>
+      <c r="C1" s="9" t="inlineStr"/>
+      <c r="D1" s="9" t="inlineStr"/>
+      <c r="E1" s="9" t="inlineStr"/>
       <c r="F1" s="9" t="n"/>
       <c r="G1" s="9" t="n"/>
       <c r="H1" s="9" t="n"/>
@@ -904,64 +940,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="8">
-      <c r="A3" s="7" t="inlineStr">
-        <is>
-          <t>20240813</t>
-        </is>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7" t="inlineStr">
-        <is>
-          <t>17673326-8</t>
-        </is>
-      </c>
-      <c r="D3" s="7" t="inlineStr">
-        <is>
-          <t>Maria Jose Rodriguez</t>
-        </is>
-      </c>
-      <c r="E3" s="7" t="inlineStr">
-        <is>
-          <t>colaco sn km3 parcela 9</t>
-        </is>
-      </c>
-      <c r="F3" s="7" t="inlineStr">
-        <is>
-          <t>ca</t>
-        </is>
-      </c>
-      <c r="G3" s="7" t="inlineStr">
-        <is>
-          <t>88809704</t>
-        </is>
-      </c>
-      <c r="H3" s="7" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="I3" s="7" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="J3" s="7" t="inlineStr">
-        <is>
-          <t>20240801</t>
-        </is>
-      </c>
-      <c r="K3" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L3" s="7" t="inlineStr">
-        <is>
-          <t>2024-09-02</t>
-        </is>
-      </c>
-    </row>
+    <row r="3" ht="15" customHeight="1" s="8"/>
     <row r="4" ht="15" customHeight="1" s="8"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -976,7 +955,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
@@ -1226,6 +1205,181 @@
       <c r="L4" s="7" t="inlineStr">
         <is>
           <t>1ca3lt</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>20240813</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>17673326-8</t>
+        </is>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>Maria Jose Rodriguez</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F5" s="7" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="G5" s="7" t="inlineStr">
+        <is>
+          <t>88809704</t>
+        </is>
+      </c>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I5" s="7" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J5" s="7" t="inlineStr">
+        <is>
+          <t>20240801</t>
+        </is>
+      </c>
+      <c r="K5" s="7" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+      <c r="L5" s="7" t="inlineStr">
+        <is>
+          <t>1ca3lt ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>20240822</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="inlineStr">
+        <is>
+          <t>15437239-7</t>
+        </is>
+      </c>
+      <c r="D6" s="7" t="inlineStr">
+        <is>
+          <t>Ishovias</t>
+        </is>
+      </c>
+      <c r="E6" s="7" t="inlineStr">
+        <is>
+          <t>cloacsoin sn</t>
+        </is>
+      </c>
+      <c r="F6" s="7" t="inlineStr">
+        <is>
+          <t>Salhued</t>
+        </is>
+      </c>
+      <c r="G6" s="7" t="inlineStr">
+        <is>
+          <t>99953274</t>
+        </is>
+      </c>
+      <c r="H6" s="7" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I6" s="7" t="inlineStr">
+        <is>
+          <t>Cliente test</t>
+        </is>
+      </c>
+      <c r="K6" s="7" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+      <c r="L6" s="7" t="inlineStr">
+        <is>
+          <t>1ca3lt ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>20240822</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D7" s="7" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E7" s="7" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F7" s="7" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G7" s="7" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H7" s="7" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I7" s="7" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J7" s="7" t="inlineStr">
+        <is>
+          <t>20240813</t>
+        </is>
+      </c>
+      <c r="K7" s="7" t="inlineStr">
+        <is>
+          <t>POSPUESTO</t>
+        </is>
+      </c>
+      <c r="L7" s="7" t="inlineStr">
+        <is>
+          <t>DEUDA</t>
         </is>
       </c>
     </row>
@@ -1315,10 +1469,39 @@
           <t>Ruta Chiloe-PtoMontt</t>
         </is>
       </c>
-      <c r="E3" s="7" t="n"/>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E3" s="7" t="inlineStr">
+        <is>
+          <t>2024-08-15T16:25:53.051404 RUTA FINALIZADA</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="8">
-      <c r="A4" s="7" t="n"/>
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>20240822</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>ruta TEST</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-08-15T16:33:29.303252 RUTA FINALIZADA</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="8">
       <c r="A5" s="7" t="n"/>

</xml_diff>

<commit_message>
Reparando boton cancelar de confpos.html
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -857,7 +857,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -878,8 +878,16 @@
           <t xml:space="preserve">Ruta actual: </t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr"/>
-      <c r="C1" s="9" t="inlineStr"/>
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>20240816</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>ruta TEST</t>
+        </is>
+      </c>
       <c r="D1" s="9" t="inlineStr"/>
       <c r="E1" s="9" t="inlineStr"/>
       <c r="F1" s="9" t="n"/>
@@ -940,7 +948,64 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="8"/>
+    <row r="3" ht="15" customHeight="1" s="8">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>20240816</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>20240813</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>120</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2024-12-01</t>
+        </is>
+      </c>
+    </row>
     <row r="4" ht="15" customHeight="1" s="8"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -1491,20 +1556,29 @@
           <t>ruta TEST</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="7" t="inlineStr">
         <is>
           <t>2024-08-15T16:33:29.303252 RUTA FINALIZADA</t>
         </is>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="8">
-      <c r="A5" s="7" t="n"/>
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>20240816</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>ruta TEST</t>
+        </is>
+      </c>
       <c r="E5" s="7" t="n"/>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="8">

</xml_diff>

<commit_message>
bug menor y ajuste de estilo confpos.html
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -730,7 +730,7 @@
       </c>
       <c r="I3" s="7" t="inlineStr">
         <is>
-          <t>20240813</t>
+          <t>2024-08-16</t>
         </is>
       </c>
       <c r="J3" s="7" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="K3" s="7" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2024-12-16</t>
         </is>
       </c>
     </row>
@@ -857,7 +857,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -878,16 +878,8 @@
           <t xml:space="preserve">Ruta actual: </t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
-        <is>
-          <t>20240816</t>
-        </is>
-      </c>
-      <c r="C1" s="9" t="inlineStr">
-        <is>
-          <t>ruta TEST</t>
-        </is>
-      </c>
+      <c r="B1" s="9" t="inlineStr"/>
+      <c r="C1" s="9" t="inlineStr"/>
       <c r="D1" s="9" t="inlineStr"/>
       <c r="E1" s="9" t="inlineStr"/>
       <c r="F1" s="9" t="n"/>
@@ -948,64 +940,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="8">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>20240816</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>16.742.249-7</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Isaias Beroiza Mora</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>colaco sn km3 parcela 9</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Calbuco</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>88809703</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>20240813</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>120</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>2024-12-01</t>
-        </is>
-      </c>
-    </row>
+    <row r="3" ht="15" customHeight="1" s="8"/>
     <row r="4" ht="15" customHeight="1" s="8"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -1020,7 +955,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
@@ -1445,6 +1380,66 @@
       <c r="L7" s="7" t="inlineStr">
         <is>
           <t>DEUDA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>20240816</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D8" s="7" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E8" s="7" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F8" s="7" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G8" s="7" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H8" s="7" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I8" s="7" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J8" s="7" t="inlineStr">
+        <is>
+          <t>20240813</t>
+        </is>
+      </c>
+      <c r="K8" s="7" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+      <c r="L8" s="7" t="inlineStr">
+        <is>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -1579,7 +1574,14 @@
           <t>ruta TEST</t>
         </is>
       </c>
-      <c r="E5" s="7" t="n"/>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7" t="inlineStr">
+        <is>
+          <t>2024-08-16T15:37:51.807710 RUTA FINALIZADA</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="8">
       <c r="A6" s="7" t="n"/>

</xml_diff>

<commit_message>
Trabajando en estilos en rutaactual para marcar a clientes con DEUDA
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -645,10 +645,14 @@
           <t>88873234</t>
         </is>
       </c>
-      <c r="G2" s="1" t="n"/>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>DEUDA</t>
         </is>
       </c>
       <c r="I2" s="1" t="n">
@@ -656,12 +660,12 @@
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>20240801</t>
+          <t>2024-08-14</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
         <is>
-          <t>2024-09-30</t>
+          <t>2024-10-15</t>
         </is>
       </c>
     </row>
@@ -703,7 +707,7 @@
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>DEUDA</t>
         </is>
       </c>
       <c r="I3" s="1" t="n">
@@ -766,12 +770,12 @@
       </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
-          <t>2024-08-29</t>
+          <t>2024-08-14</t>
         </is>
       </c>
       <c r="K4" s="1" t="inlineStr">
         <is>
-          <t>2024-09-30</t>
+          <t>2024-09-15</t>
         </is>
       </c>
     </row>
@@ -834,7 +838,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
@@ -855,8 +859,16 @@
           <t xml:space="preserve">Ruta actual: </t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr"/>
-      <c r="C1" s="2" t="inlineStr"/>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>20240824</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Test4</t>
+        </is>
+      </c>
       <c r="D1" s="2" t="inlineStr"/>
       <c r="E1" s="2" t="inlineStr"/>
       <c r="F1" s="2" t="n"/>
@@ -917,8 +929,231 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="8"/>
-    <row r="4" ht="15" customHeight="1" s="8"/>
+    <row r="3" ht="15" customHeight="1" s="8">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>20240824</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>17234876-8</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>Sigo</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>Kosovo</t>
+        </is>
+      </c>
+      <c r="F3" s="0" t="inlineStr">
+        <is>
+          <t>Cloac</t>
+        </is>
+      </c>
+      <c r="G3" s="0" t="inlineStr">
+        <is>
+          <t>88873234</t>
+        </is>
+      </c>
+      <c r="H3" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I3" s="0" t="inlineStr">
+        <is>
+          <t>DEUDA</t>
+        </is>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="K3" s="0" t="inlineStr">
+        <is>
+          <t>2024-08-14</t>
+        </is>
+      </c>
+      <c r="L3" s="0" t="inlineStr">
+        <is>
+          <t>2024-10-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="8">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>20240824</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H4" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t>DEUDA</t>
+        </is>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="K4" s="0" t="inlineStr">
+        <is>
+          <t>2024-08-29</t>
+        </is>
+      </c>
+      <c r="L4" s="0" t="inlineStr">
+        <is>
+          <t>2024-12-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>20240824</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>17673326-8</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>Maria Jose Rodriguez</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="G5" s="0" t="inlineStr">
+        <is>
+          <t>88809704</t>
+        </is>
+      </c>
+      <c r="H5" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I5" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="K5" s="0" t="inlineStr">
+        <is>
+          <t>2024-08-14</t>
+        </is>
+      </c>
+      <c r="L5" s="0" t="inlineStr">
+        <is>
+          <t>2024-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>20240824</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>15437239-7</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Ishovias</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>cloacsoin sn</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Salhued</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>99953274</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Cliente test</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2024-08-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
 </worksheet>
@@ -930,7 +1165,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
@@ -1580,6 +1815,346 @@
       <c r="L11" s="0" t="inlineStr">
         <is>
           <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>20240814</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>17234876-8</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>Sigo</t>
+        </is>
+      </c>
+      <c r="E12" s="0" t="inlineStr">
+        <is>
+          <t>Kosovo</t>
+        </is>
+      </c>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>Cloac</t>
+        </is>
+      </c>
+      <c r="G12" s="0" t="inlineStr">
+        <is>
+          <t>88873234</t>
+        </is>
+      </c>
+      <c r="I12" s="0" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="K12" s="0" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+      <c r="L12" s="0" t="inlineStr">
+        <is>
+          <t>3ca3lt ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>20240814</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E13" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F13" s="0" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G13" s="0" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H13" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I13" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="K13" s="0" t="inlineStr">
+        <is>
+          <t>POSPUESTO</t>
+        </is>
+      </c>
+      <c r="L13" s="0" t="inlineStr">
+        <is>
+          <t>DEUDA</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>20240814</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>17673326-8</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>Maria Jose Rodriguez</t>
+        </is>
+      </c>
+      <c r="E14" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F14" s="0" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="G14" s="0" t="inlineStr">
+        <is>
+          <t>88809704</t>
+        </is>
+      </c>
+      <c r="H14" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I14" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="K14" s="0" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+      <c r="L14" s="0" t="inlineStr">
+        <is>
+          <t>3ca3lt 1ba</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>20240814</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>15437239-7</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>Ishovias</t>
+        </is>
+      </c>
+      <c r="E15" s="0" t="inlineStr">
+        <is>
+          <t>cloacsoin sn</t>
+        </is>
+      </c>
+      <c r="F15" s="0" t="inlineStr">
+        <is>
+          <t>Salhued</t>
+        </is>
+      </c>
+      <c r="G15" s="0" t="inlineStr">
+        <is>
+          <t>99953274</t>
+        </is>
+      </c>
+      <c r="H15" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I15" s="0" t="inlineStr">
+        <is>
+          <t>Cliente test</t>
+        </is>
+      </c>
+      <c r="K15" s="0" t="inlineStr">
+        <is>
+          <t>POSPUESTO</t>
+        </is>
+      </c>
+      <c r="L15" s="0" t="inlineStr">
+        <is>
+          <t>DEUDA</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>20240812</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="E16" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="G16" s="0" t="inlineStr">
+        <is>
+          <t>88809703</t>
+        </is>
+      </c>
+      <c r="H16" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I16" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="K16" s="0" t="inlineStr">
+        <is>
+          <t>POSPUESTO</t>
+        </is>
+      </c>
+      <c r="L16" s="0" t="inlineStr">
+        <is>
+          <t>Deuda</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>20240812</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>17673326-8</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>Maria Jose Rodriguez</t>
+        </is>
+      </c>
+      <c r="E17" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="G17" s="0" t="inlineStr">
+        <is>
+          <t>88809704</t>
+        </is>
+      </c>
+      <c r="H17" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I17" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="K17" s="0" t="inlineStr">
+        <is>
+          <t>POSPUESTO</t>
+        </is>
+      </c>
+      <c r="L17" s="0" t="inlineStr">
+        <is>
+          <t>DEUDA</t>
         </is>
       </c>
     </row>
@@ -1732,27 +2307,77 @@
           <t>ruta ejemplo</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="0" t="inlineStr">
         <is>
           <t>2024-08-21T13:02:54.651073 RUTA FINALIZADA</t>
         </is>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="8">
-      <c r="A7" s="1" t="n"/>
-      <c r="C7" s="1" t="n"/>
-      <c r="E7" s="1" t="n"/>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>20240814</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>Ruta demo</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
+          <t>2024-08-23T16:13:38.501669 RUTA FINALIZADA</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="8">
-      <c r="A8" s="1" t="n"/>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>20240812</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>Ruta test3</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>2024-08-23T16:31:10.901471 RUTA FINALIZADA</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="8">
-      <c r="A9" s="1" t="n"/>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>20240824</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>Test4</t>
+        </is>
+      </c>
       <c r="E9" s="1" t="n"/>
     </row>
     <row r="10" ht="13.5" customHeight="1" s="8">

</xml_diff>

<commit_message>
Agregando autorizacion por privilegios
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="usuarios" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <sz val="11"/>
@@ -35,6 +35,10 @@
       <name val="Calibri"/>
       <charset val="1"/>
       <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -65,7 +69,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -85,7 +89,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -463,8 +467,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
@@ -518,12 +522,12 @@
     <row r="4" ht="15" customHeight="1" s="8">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>mauricio</t>
+          <t>invitado</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>1n9v0w5r@x2o9v$zzm1n$zS&amp;v#5r@x5rYl</t>
+          <t>5IzmR?5IT%$Z0wYL</t>
         </is>
       </c>
     </row>
@@ -645,14 +649,10 @@
           <t>88873234</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="G2" s="1" t="n"/>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>DEUDA</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="I2" s="1" t="n">
@@ -660,12 +660,12 @@
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>2024-08-14</t>
+          <t>20240801</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
         <is>
-          <t>2024-10-15</t>
+          <t>2024-09-30</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
-          <t>DEUDA</t>
+          <t>ok</t>
         </is>
       </c>
       <c r="I3" s="1" t="n">
@@ -770,12 +770,12 @@
       </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
-          <t>2024-08-14</t>
+          <t>2024-08-29</t>
         </is>
       </c>
       <c r="K4" s="1" t="inlineStr">
         <is>
-          <t>2024-09-15</t>
+          <t>2024-09-30</t>
         </is>
       </c>
     </row>
@@ -838,9 +838,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -859,16 +859,8 @@
           <t xml:space="preserve">Ruta actual: </t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>20240824</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Test4</t>
-        </is>
-      </c>
+      <c r="B1" s="2" t="inlineStr"/>
+      <c r="C1" s="2" t="inlineStr"/>
       <c r="D1" s="2" t="inlineStr"/>
       <c r="E1" s="2" t="inlineStr"/>
       <c r="F1" s="2" t="n"/>
@@ -929,231 +921,8 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="8">
-      <c r="A3" s="0" t="inlineStr">
-        <is>
-          <t>20240824</t>
-        </is>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>17234876-8</t>
-        </is>
-      </c>
-      <c r="D3" s="0" t="inlineStr">
-        <is>
-          <t>Sigo</t>
-        </is>
-      </c>
-      <c r="E3" s="0" t="inlineStr">
-        <is>
-          <t>Kosovo</t>
-        </is>
-      </c>
-      <c r="F3" s="0" t="inlineStr">
-        <is>
-          <t>Cloac</t>
-        </is>
-      </c>
-      <c r="G3" s="0" t="inlineStr">
-        <is>
-          <t>88873234</t>
-        </is>
-      </c>
-      <c r="H3" s="0" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I3" s="0" t="inlineStr">
-        <is>
-          <t>DEUDA</t>
-        </is>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="K3" s="0" t="inlineStr">
-        <is>
-          <t>2024-08-14</t>
-        </is>
-      </c>
-      <c r="L3" s="0" t="inlineStr">
-        <is>
-          <t>2024-10-15</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1" s="8">
-      <c r="A4" s="0" t="inlineStr">
-        <is>
-          <t>20240824</t>
-        </is>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>16.742.249-7</t>
-        </is>
-      </c>
-      <c r="D4" s="0" t="inlineStr">
-        <is>
-          <t>Isaias Beroiza Mora</t>
-        </is>
-      </c>
-      <c r="E4" s="0" t="inlineStr">
-        <is>
-          <t>colaco sn km3 parcela 9</t>
-        </is>
-      </c>
-      <c r="F4" s="0" t="inlineStr">
-        <is>
-          <t>Calbuco</t>
-        </is>
-      </c>
-      <c r="G4" s="0" t="inlineStr">
-        <is>
-          <t>88809703</t>
-        </is>
-      </c>
-      <c r="H4" s="0" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="I4" s="0" t="inlineStr">
-        <is>
-          <t>DEUDA</t>
-        </is>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="K4" s="0" t="inlineStr">
-        <is>
-          <t>2024-08-29</t>
-        </is>
-      </c>
-      <c r="L4" s="0" t="inlineStr">
-        <is>
-          <t>2024-12-29</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="inlineStr">
-        <is>
-          <t>20240824</t>
-        </is>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="0" t="inlineStr">
-        <is>
-          <t>17673326-8</t>
-        </is>
-      </c>
-      <c r="D5" s="0" t="inlineStr">
-        <is>
-          <t>Maria Jose Rodriguez</t>
-        </is>
-      </c>
-      <c r="E5" s="0" t="inlineStr">
-        <is>
-          <t>colaco sn km3 parcela 9</t>
-        </is>
-      </c>
-      <c r="F5" s="0" t="inlineStr">
-        <is>
-          <t>ca</t>
-        </is>
-      </c>
-      <c r="G5" s="0" t="inlineStr">
-        <is>
-          <t>88809704</t>
-        </is>
-      </c>
-      <c r="H5" s="0" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="I5" s="0" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K5" s="0" t="inlineStr">
-        <is>
-          <t>2024-08-14</t>
-        </is>
-      </c>
-      <c r="L5" s="0" t="inlineStr">
-        <is>
-          <t>2024-09-15</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>20240824</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>4</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>15437239-7</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Ishovias</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>cloacsoin sn</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Salhued</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>99953274</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Cliente test</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>2024-08-22</t>
-        </is>
-      </c>
-    </row>
-    <row r="7"/>
+    <row r="3" ht="15" customHeight="1" s="8"/>
+    <row r="4" ht="15" customHeight="1" s="8"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
 </worksheet>
@@ -1165,7 +934,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
@@ -1712,447 +1481,107 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>20240829</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>17673326-8</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>Maria Jose Rodriguez</t>
+        </is>
+      </c>
+      <c r="E10" s="0" t="inlineStr">
+        <is>
+          <t>colaco sn km3 parcela 9</t>
+        </is>
+      </c>
+      <c r="F10" s="0" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="G10" s="0" t="inlineStr">
+        <is>
+          <t>88809704</t>
+        </is>
+      </c>
+      <c r="H10" s="0" t="inlineStr">
+        <is>
+          <t>por buscar</t>
+        </is>
+      </c>
+      <c r="I10" s="0" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="K10" s="0" t="inlineStr">
+        <is>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+      <c r="L10" s="0" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
         <v>20240829</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B11" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C11" s="0" t="n">
         <v>154322347</v>
       </c>
-      <c r="D10" s="0" t="inlineStr">
+      <c r="D11" s="0" t="inlineStr">
         <is>
           <t>kalfore</t>
         </is>
       </c>
-      <c r="E10" s="0" t="inlineStr">
+      <c r="E11" s="0" t="inlineStr">
         <is>
           <t>jehsol</t>
         </is>
       </c>
-      <c r="F10" s="0" t="inlineStr">
+      <c r="F11" s="0" t="inlineStr">
         <is>
           <t>ushsk</t>
         </is>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G11" s="0" t="n">
         <v>25698323</v>
       </c>
-      <c r="H10" s="0" t="inlineStr">
+      <c r="H11" s="0" t="inlineStr">
         <is>
           <t xml:space="preserve">por buscar </t>
         </is>
       </c>
-      <c r="I10" s="0" t="inlineStr">
+      <c r="I11" s="0" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
       </c>
-      <c r="K10" s="0" t="inlineStr">
-        <is>
-          <t>REALIZADO</t>
-        </is>
-      </c>
-      <c r="L10" s="0" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" s="0" t="inlineStr">
-        <is>
-          <t>17673326-8</t>
-        </is>
-      </c>
-      <c r="D11" s="0" t="inlineStr">
-        <is>
-          <t>Maria Jose Rodriguez</t>
-        </is>
-      </c>
-      <c r="E11" s="0" t="inlineStr">
-        <is>
-          <t>colaco sn km3 parcela 9</t>
-        </is>
-      </c>
-      <c r="F11" s="0" t="inlineStr">
-        <is>
-          <t>ca</t>
-        </is>
-      </c>
-      <c r="G11" s="0" t="inlineStr">
-        <is>
-          <t>88809704</t>
-        </is>
-      </c>
-      <c r="H11" s="0" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="I11" s="0" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>30</v>
-      </c>
       <c r="K11" s="0" t="inlineStr">
         <is>
-          <t>REALIZADO</t>
+          <t>POSPUESTO</t>
         </is>
       </c>
       <c r="L11" s="0" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0" t="inlineStr">
-        <is>
-          <t>20240814</t>
-        </is>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="0" t="inlineStr">
-        <is>
-          <t>17234876-8</t>
-        </is>
-      </c>
-      <c r="D12" s="0" t="inlineStr">
-        <is>
-          <t>Sigo</t>
-        </is>
-      </c>
-      <c r="E12" s="0" t="inlineStr">
-        <is>
-          <t>Kosovo</t>
-        </is>
-      </c>
-      <c r="F12" s="0" t="inlineStr">
-        <is>
-          <t>Cloac</t>
-        </is>
-      </c>
-      <c r="G12" s="0" t="inlineStr">
-        <is>
-          <t>88873234</t>
-        </is>
-      </c>
-      <c r="I12" s="0" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="K12" s="0" t="inlineStr">
-        <is>
-          <t>REALIZADO</t>
-        </is>
-      </c>
-      <c r="L12" s="0" t="inlineStr">
-        <is>
-          <t>3ca3lt ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="0" t="inlineStr">
-        <is>
-          <t>20240814</t>
-        </is>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" s="0" t="inlineStr">
-        <is>
-          <t>16.742.249-7</t>
-        </is>
-      </c>
-      <c r="D13" s="0" t="inlineStr">
-        <is>
-          <t>Isaias Beroiza Mora</t>
-        </is>
-      </c>
-      <c r="E13" s="0" t="inlineStr">
-        <is>
-          <t>colaco sn km3 parcela 9</t>
-        </is>
-      </c>
-      <c r="F13" s="0" t="inlineStr">
-        <is>
-          <t>Calbuco</t>
-        </is>
-      </c>
-      <c r="G13" s="0" t="inlineStr">
-        <is>
-          <t>88809703</t>
-        </is>
-      </c>
-      <c r="H13" s="0" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="I13" s="0" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="K13" s="0" t="inlineStr">
-        <is>
-          <t>POSPUESTO</t>
-        </is>
-      </c>
-      <c r="L13" s="0" t="inlineStr">
-        <is>
-          <t>DEUDA</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="0" t="inlineStr">
-        <is>
-          <t>20240814</t>
-        </is>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C14" s="0" t="inlineStr">
-        <is>
-          <t>17673326-8</t>
-        </is>
-      </c>
-      <c r="D14" s="0" t="inlineStr">
-        <is>
-          <t>Maria Jose Rodriguez</t>
-        </is>
-      </c>
-      <c r="E14" s="0" t="inlineStr">
-        <is>
-          <t>colaco sn km3 parcela 9</t>
-        </is>
-      </c>
-      <c r="F14" s="0" t="inlineStr">
-        <is>
-          <t>ca</t>
-        </is>
-      </c>
-      <c r="G14" s="0" t="inlineStr">
-        <is>
-          <t>88809704</t>
-        </is>
-      </c>
-      <c r="H14" s="0" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="I14" s="0" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K14" s="0" t="inlineStr">
-        <is>
-          <t>REALIZADO</t>
-        </is>
-      </c>
-      <c r="L14" s="0" t="inlineStr">
-        <is>
-          <t>3ca3lt 1ba</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="0" t="inlineStr">
-        <is>
-          <t>20240814</t>
-        </is>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C15" s="0" t="inlineStr">
-        <is>
-          <t>15437239-7</t>
-        </is>
-      </c>
-      <c r="D15" s="0" t="inlineStr">
-        <is>
-          <t>Ishovias</t>
-        </is>
-      </c>
-      <c r="E15" s="0" t="inlineStr">
-        <is>
-          <t>cloacsoin sn</t>
-        </is>
-      </c>
-      <c r="F15" s="0" t="inlineStr">
-        <is>
-          <t>Salhued</t>
-        </is>
-      </c>
-      <c r="G15" s="0" t="inlineStr">
-        <is>
-          <t>99953274</t>
-        </is>
-      </c>
-      <c r="H15" s="0" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="I15" s="0" t="inlineStr">
-        <is>
-          <t>Cliente test</t>
-        </is>
-      </c>
-      <c r="K15" s="0" t="inlineStr">
-        <is>
-          <t>POSPUESTO</t>
-        </is>
-      </c>
-      <c r="L15" s="0" t="inlineStr">
-        <is>
-          <t>DEUDA</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="0" t="inlineStr">
-        <is>
-          <t>20240812</t>
-        </is>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="0" t="inlineStr">
-        <is>
-          <t>16.742.249-7</t>
-        </is>
-      </c>
-      <c r="D16" s="0" t="inlineStr">
-        <is>
-          <t>Isaias Beroiza Mora</t>
-        </is>
-      </c>
-      <c r="E16" s="0" t="inlineStr">
-        <is>
-          <t>colaco sn km3 parcela 9</t>
-        </is>
-      </c>
-      <c r="F16" s="0" t="inlineStr">
-        <is>
-          <t>Calbuco</t>
-        </is>
-      </c>
-      <c r="G16" s="0" t="inlineStr">
-        <is>
-          <t>88809703</t>
-        </is>
-      </c>
-      <c r="H16" s="0" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="I16" s="0" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="K16" s="0" t="inlineStr">
-        <is>
-          <t>POSPUESTO</t>
-        </is>
-      </c>
-      <c r="L16" s="0" t="inlineStr">
-        <is>
-          <t>Deuda</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="0" t="inlineStr">
-        <is>
-          <t>20240812</t>
-        </is>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C17" s="0" t="inlineStr">
-        <is>
-          <t>17673326-8</t>
-        </is>
-      </c>
-      <c r="D17" s="0" t="inlineStr">
-        <is>
-          <t>Maria Jose Rodriguez</t>
-        </is>
-      </c>
-      <c r="E17" s="0" t="inlineStr">
-        <is>
-          <t>colaco sn km3 parcela 9</t>
-        </is>
-      </c>
-      <c r="F17" s="0" t="inlineStr">
-        <is>
-          <t>ca</t>
-        </is>
-      </c>
-      <c r="G17" s="0" t="inlineStr">
-        <is>
-          <t>88809704</t>
-        </is>
-      </c>
-      <c r="H17" s="0" t="inlineStr">
-        <is>
-          <t>por buscar</t>
-        </is>
-      </c>
-      <c r="I17" s="0" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="J17" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K17" s="0" t="inlineStr">
-        <is>
-          <t>POSPUESTO</t>
-        </is>
-      </c>
-      <c r="L17" s="0" t="inlineStr">
         <is>
           <t>DEUDA</t>
         </is>
@@ -2307,77 +1736,30 @@
           <t>ruta ejemplo</t>
         </is>
       </c>
-      <c r="C6" s="0" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E6" s="0" t="inlineStr">
-        <is>
-          <t>2024-08-21T13:02:54.651073 RUTA FINALIZADA</t>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2024-08-24T14:23:47.565847 RUTA FINALIZADA</t>
         </is>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="8">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>20240814</t>
-        </is>
-      </c>
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>Ruta demo</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D7" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E7" s="1" t="inlineStr">
-        <is>
-          <t>2024-08-23T16:13:38.501669 RUTA FINALIZADA</t>
-        </is>
-      </c>
+      <c r="A7" s="1" t="n"/>
+      <c r="C7" s="1" t="n"/>
+      <c r="E7" s="1" t="n"/>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>20240812</t>
-        </is>
-      </c>
-      <c r="B8" s="0" t="inlineStr">
-        <is>
-          <t>Ruta test3</t>
-        </is>
-      </c>
-      <c r="D8" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E8" s="0" t="inlineStr">
-        <is>
-          <t>2024-08-23T16:31:10.901471 RUTA FINALIZADA</t>
-        </is>
-      </c>
+      <c r="A8" s="1" t="n"/>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="8">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>20240824</t>
-        </is>
-      </c>
-      <c r="B9" s="0" t="inlineStr">
-        <is>
-          <t>Test4</t>
-        </is>
-      </c>
+      <c r="A9" s="1" t="n"/>
       <c r="E9" s="1" t="n"/>
     </row>
     <row r="10" ht="13.5" customHeight="1" s="8">

</xml_diff>

<commit_message>
Refactorizando 43% (confpos cliente nuevo)
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -624,7 +624,7 @@
       </c>
       <c r="C2" s="18" t="inlineStr">
         <is>
-          <t>YgdOanf8gUjOmbd6zT$m</t>
+          <t>qh#dpd52lf8gcqSTYTj0</t>
         </is>
       </c>
     </row>
@@ -1407,7 +1407,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L89"/>
+  <dimension ref="A1:K87"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1456,8 +1456,14 @@
       <c r="K1" s="23" t="n"/>
     </row>
     <row r="2" ht="13.5" customHeight="1" s="16">
-      <c r="A2" s="23" t="n"/>
-      <c r="B2" s="23" t="n"/>
+      <c r="A2" s="23" t="n">
+        <v>20250310</v>
+      </c>
+      <c r="B2" s="23" t="inlineStr">
+        <is>
+          <t>Ruta de ejemplo de importacion</t>
+        </is>
+      </c>
       <c r="D2" s="23" t="n"/>
       <c r="G2" s="23" t="n"/>
       <c r="H2" s="23" t="n"/>
@@ -1486,7 +1492,6 @@
       <c r="K4" s="23" t="n"/>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="16">
-      <c r="A5" s="23" t="n"/>
       <c r="B5" s="23" t="n"/>
       <c r="D5" s="23" t="n"/>
       <c r="G5" s="23" t="n"/>
@@ -1496,7 +1501,6 @@
       <c r="K5" s="23" t="n"/>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="16">
-      <c r="A6" s="23" t="n"/>
       <c r="B6" s="23" t="n"/>
       <c r="D6" s="23" t="n"/>
       <c r="G6" s="23" t="n"/>
@@ -2234,24 +2238,8 @@
       <c r="J87" s="23" t="n"/>
       <c r="K87" s="23" t="n"/>
     </row>
-    <row r="88" ht="15.75" customHeight="1" s="16">
-      <c r="B88" s="23" t="n"/>
-      <c r="D88" s="23" t="n"/>
-      <c r="G88" s="23" t="n"/>
-      <c r="H88" s="23" t="n"/>
-      <c r="I88" s="23" t="n"/>
-      <c r="J88" s="23" t="n"/>
-      <c r="K88" s="23" t="n"/>
-    </row>
-    <row r="89" ht="15.75" customHeight="1" s="16">
-      <c r="B89" s="23" t="n"/>
-      <c r="D89" s="23" t="n"/>
-      <c r="G89" s="23" t="n"/>
-      <c r="H89" s="23" t="n"/>
-      <c r="I89" s="23" t="n"/>
-      <c r="J89" s="23" t="n"/>
-      <c r="K89" s="23" t="n"/>
-    </row>
+    <row r="88" ht="15.75" customHeight="1" s="16"/>
+    <row r="89" ht="15.75" customHeight="1" s="16"/>
     <row r="90" ht="15.75" customHeight="1" s="16"/>
     <row r="91" ht="15.75" customHeight="1" s="16"/>
     <row r="92" ht="15.75" customHeight="1" s="16"/>

</xml_diff>

<commit_message>
Refactorizando 44% (confpos cliente testing)
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -624,7 +624,7 @@
       </c>
       <c r="C2" s="18" t="inlineStr">
         <is>
-          <t>qh#dpd52lf8gcqSTYTj0</t>
+          <t>cf@6pXX034calbd4zd1X</t>
         </is>
       </c>
     </row>
@@ -1407,7 +1407,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:K87"/>
+  <dimension ref="A1:K86"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1457,11 +1457,11 @@
     </row>
     <row r="2" ht="13.5" customHeight="1" s="16">
       <c r="A2" s="23" t="n">
-        <v>20250310</v>
+        <v>20250318</v>
       </c>
       <c r="B2" s="23" t="inlineStr">
         <is>
-          <t>Ruta de ejemplo de importacion</t>
+          <t>Ruta de ejemplo PTO MONTT</t>
         </is>
       </c>
       <c r="D2" s="23" t="n"/>
@@ -1482,7 +1482,6 @@
       <c r="K3" s="23" t="n"/>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="16">
-      <c r="A4" s="23" t="n"/>
       <c r="B4" s="23" t="n"/>
       <c r="D4" s="23" t="n"/>
       <c r="G4" s="23" t="n"/>
@@ -2229,15 +2228,7 @@
       <c r="J86" s="23" t="n"/>
       <c r="K86" s="23" t="n"/>
     </row>
-    <row r="87" ht="15.75" customHeight="1" s="16">
-      <c r="B87" s="23" t="n"/>
-      <c r="D87" s="23" t="n"/>
-      <c r="G87" s="23" t="n"/>
-      <c r="H87" s="23" t="n"/>
-      <c r="I87" s="23" t="n"/>
-      <c r="J87" s="23" t="n"/>
-      <c r="K87" s="23" t="n"/>
-    </row>
+    <row r="87" ht="15.75" customHeight="1" s="16"/>
     <row r="88" ht="15.75" customHeight="1" s="16"/>
     <row r="89" ht="15.75" customHeight="1" s="16"/>
     <row r="90" ht="15.75" customHeight="1" s="16"/>

</xml_diff>

<commit_message>
Agregando nueva vista de rutaactual
Nueva vista que permite poder ver datos en forma de <ul> mas comodo para dispositivos moviles
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -540,7 +540,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>AQ1_YbH59t4udBuwF2N8aH2FIBur9tXqwQN8c9ppF9s</t>
+          <t>3ydOcyyhuDRUfPw9hbMH2ECmblC2LPPEdcCJp06uy1A</t>
         </is>
       </c>
       <c r="D2" s="2" t="n"/>
@@ -26054,7 +26054,12 @@
       </c>
       <c r="K201" t="inlineStr">
         <is>
-          <t>enruta</t>
+          <t>REALIZADO</t>
+        </is>
+      </c>
+      <c r="L201" t="inlineStr">
+        <is>
+          <t>retiro ok</t>
         </is>
       </c>
       <c r="AI201" t="inlineStr">
@@ -26366,46 +26371,41 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>30</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>77.923.484-3</t>
+          <t>9999</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>Quiero Frenillos Osorno spa.</t>
+          <t>ACHS Rio Bueno</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>o´higgins 743 block 2p</t>
+          <t>Independencia Nº970</t>
         </is>
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Osorno</t>
+          <t>Rio bueno</t>
         </is>
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>978983247/923860996</t>
-        </is>
-      </c>
-      <c r="I207" t="inlineStr">
-        <is>
-          <t>deuda u otro problema</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J207" t="n">
-        <v>10013</v>
+        <v>10021</v>
       </c>
       <c r="K207" t="inlineStr">
         <is>
@@ -26426,7 +26426,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -26441,17 +26441,17 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>ACHS Rio Bueno</t>
+          <t>ACHS LA UNION</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>Independencia Nº970</t>
+          <t>Comercio Nº260, La Unión</t>
         </is>
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Rio bueno</t>
+          <t>La Union</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
@@ -26460,7 +26460,7 @@
         </is>
       </c>
       <c r="J208" t="n">
-        <v>10021</v>
+        <v>10020</v>
       </c>
       <c r="K208" t="inlineStr">
         <is>
@@ -26481,7 +26481,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -26491,31 +26491,36 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>9999</t>
+          <t>77.149.769-1</t>
         </is>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>ACHS LA UNION</t>
+          <t>Medic Home spa</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>Comercio Nº260, La Unión</t>
+          <t>condominio doña ines , parc 40</t>
         </is>
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>La Union</t>
+          <t>Valdivia</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>988108996</t>
+        </is>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>AVISADO</t>
         </is>
       </c>
       <c r="J209" t="n">
-        <v>10020</v>
+        <v>10023</v>
       </c>
       <c r="K209" t="inlineStr">
         <is>
@@ -26536,17 +26541,17 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>360</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>77.149.769-1</t>
+          <t>77.149.769-2</t>
         </is>
       </c>
       <c r="E210" t="inlineStr">
@@ -26556,7 +26561,7 @@
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t>condominio doña ines , parc 40</t>
+          <t>bombero Hernandez 224</t>
         </is>
       </c>
       <c r="G210" t="inlineStr">
@@ -26566,12 +26571,12 @@
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>988108996</t>
+          <t>961074516</t>
         </is>
       </c>
       <c r="I210" t="inlineStr">
         <is>
-          <t>AVISADO</t>
+          <t>retiro unico aprox 12 a 13 C /avisar cuando salga de osorno</t>
         </is>
       </c>
       <c r="J210" t="n">
@@ -26596,27 +26601,27 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>30</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>77.149.769-2</t>
+          <t>77.156.579-4</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>Medic Home spa</t>
+          <t>virtos dos spa.</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t>bombero Hernandez 224</t>
+          <t>los alamos 1121,block A dep803</t>
         </is>
       </c>
       <c r="G211" t="inlineStr">
@@ -26626,16 +26631,16 @@
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>961074516</t>
+          <t>998833928</t>
         </is>
       </c>
       <c r="I211" t="inlineStr">
         <is>
-          <t>retiro unico aprox 12 a 13 C /avisar cuando salga de osorno</t>
+          <t>FAENA /todo el dia</t>
         </is>
       </c>
       <c r="J211" t="n">
-        <v>10023</v>
+        <v>10174</v>
       </c>
       <c r="K211" t="inlineStr">
         <is>
@@ -26656,27 +26661,27 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>77.156.579-4</t>
+          <t>77.512.587-k</t>
         </is>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>virtos dos spa.</t>
+          <t>maria jo beauty estudio</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>los alamos 1121,block A dep803</t>
+          <t>janequeo 368</t>
         </is>
       </c>
       <c r="G212" t="inlineStr">
@@ -26686,16 +26691,16 @@
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>998833928</t>
+          <t>972955740</t>
         </is>
       </c>
       <c r="I212" t="inlineStr">
         <is>
-          <t>FAENA /todo el dia</t>
+          <t>9:30 a 19:30</t>
         </is>
       </c>
       <c r="J212" t="n">
-        <v>10174</v>
+        <v>10175</v>
       </c>
       <c r="K212" t="inlineStr">
         <is>
@@ -26716,7 +26721,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -26726,17 +26731,17 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>77.512.587-k</t>
+          <t>77.018.398-7</t>
         </is>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>maria jo beauty estudio</t>
+          <t>clinica estetica doc. Claudio Villegas</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
         <is>
-          <t>janequeo 368</t>
+          <t>yungay 783</t>
         </is>
       </c>
       <c r="G213" t="inlineStr">
@@ -26746,16 +26751,16 @@
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>972955740</t>
+          <t>988319274/949287402</t>
         </is>
       </c>
       <c r="I213" t="inlineStr">
         <is>
-          <t>9:30 a 19:30</t>
+          <t>10 A 13:30 A 14:30 A 18</t>
         </is>
       </c>
       <c r="J213" t="n">
-        <v>10175</v>
+        <v>10138</v>
       </c>
       <c r="K213" t="inlineStr">
         <is>
@@ -26776,27 +26781,27 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>15</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>77.018.398-7</t>
+          <t>9999</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>clinica estetica doc. Claudio Villegas</t>
+          <t>ACHS VALDIVIA</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>yungay 783</t>
+          <t>Beauchef Nº705, Valdivia</t>
         </is>
       </c>
       <c r="G214" t="inlineStr">
@@ -26806,16 +26811,11 @@
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>988319274/949287402</t>
-        </is>
-      </c>
-      <c r="I214" t="inlineStr">
-        <is>
-          <t>10 A 13:30 A 14:30 A 18</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J214" t="n">
-        <v>10138</v>
+        <v>10036</v>
       </c>
       <c r="K214" t="inlineStr">
         <is>
@@ -26836,27 +26836,27 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>17</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>9999</t>
+          <t>76.209.597-1</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>ACHS VALDIVIA</t>
+          <t>Medodonta Spa</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>Beauchef Nº705, Valdivia</t>
+          <t>Manuel Montt 0253</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
@@ -26866,11 +26866,16 @@
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>998295798</t>
+        </is>
+      </c>
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>14 a 17,30</t>
         </is>
       </c>
       <c r="J215" t="n">
-        <v>10036</v>
+        <v>10176</v>
       </c>
       <c r="K215" t="inlineStr">
         <is>
@@ -26891,27 +26896,27 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>30</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>76.209.597-1</t>
+          <t>70.362.000-0</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>Medodonta Spa</t>
+          <t>Corporación para la nutrición infantil</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>Manuel Montt 0253</t>
+          <t>Ruben Dario 285, El laurel</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
@@ -26921,16 +26926,16 @@
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>998295798</t>
+          <t>988612484</t>
         </is>
       </c>
       <c r="I216" t="inlineStr">
         <is>
-          <t>14 a 17,30</t>
+          <t>suspendido desde santiago</t>
         </is>
       </c>
       <c r="J216" t="n">
-        <v>10176</v>
+        <v>10147</v>
       </c>
       <c r="K216" t="inlineStr">
         <is>
@@ -26951,27 +26956,27 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>70.362.000-0</t>
+          <t>77.800.823-8</t>
         </is>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>Corporación para la nutrición infantil</t>
+          <t>Clinica Hora Dental</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>Ruben Dario 285, El laurel</t>
+          <t>Ramon Picarte 2629</t>
         </is>
       </c>
       <c r="G217" t="inlineStr">
@@ -26981,16 +26986,16 @@
       </c>
       <c r="H217" t="inlineStr">
         <is>
-          <t>988612484</t>
+          <t>999197935</t>
         </is>
       </c>
       <c r="I217" t="inlineStr">
         <is>
-          <t>suspendido desde santiago</t>
+          <t>deuda u otro problema</t>
         </is>
       </c>
       <c r="J217" t="n">
-        <v>10147</v>
+        <v>10177</v>
       </c>
       <c r="K217" t="inlineStr">
         <is>
@@ -27011,7 +27016,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -27021,17 +27026,17 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>77.800.823-8</t>
+          <t>77.624.403-1</t>
         </is>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>Clinica Hora Dental</t>
+          <t>serv para salud humana Gloria Jofré EIRL</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>Ramon Picarte 2629</t>
+          <t>García Reyes 686</t>
         </is>
       </c>
       <c r="G218" t="inlineStr">
@@ -27041,7 +27046,7 @@
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>999197935</t>
+          <t>952541245</t>
         </is>
       </c>
       <c r="I218" t="inlineStr">
@@ -27050,7 +27055,7 @@
         </is>
       </c>
       <c r="J218" t="n">
-        <v>10177</v>
+        <v>10178</v>
       </c>
       <c r="K218" t="inlineStr">
         <is>
@@ -27063,66 +27068,7 @@
         </is>
       </c>
     </row>
-    <row r="219">
-      <c r="A219" t="inlineStr">
-        <is>
-          <t>20250804</t>
-        </is>
-      </c>
-      <c r="B219" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="C219" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-      <c r="D219" t="inlineStr">
-        <is>
-          <t>77.624.403-1</t>
-        </is>
-      </c>
-      <c r="E219" t="inlineStr">
-        <is>
-          <t>serv para salud humana Gloria Jofré EIRL</t>
-        </is>
-      </c>
-      <c r="F219" t="inlineStr">
-        <is>
-          <t>García Reyes 686</t>
-        </is>
-      </c>
-      <c r="G219" t="inlineStr">
-        <is>
-          <t>Valdivia</t>
-        </is>
-      </c>
-      <c r="H219" t="inlineStr">
-        <is>
-          <t>952541245</t>
-        </is>
-      </c>
-      <c r="I219" t="inlineStr">
-        <is>
-          <t>deuda u otro problema</t>
-        </is>
-      </c>
-      <c r="J219" t="n">
-        <v>10178</v>
-      </c>
-      <c r="K219" t="inlineStr">
-        <is>
-          <t>enruta</t>
-        </is>
-      </c>
-      <c r="AI219" t="inlineStr">
-        <is>
-          <t>Osorno-RioBueno-LaUnion-Valdivia</t>
-        </is>
-      </c>
-    </row>
+    <row r="219"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -27981,7 +27927,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X140"/>
+  <dimension ref="A1:X141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
@@ -30060,6 +30006,16 @@
       </c>
       <c r="B140" t="n">
         <v>10169</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>20250804</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>10017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregando sistema en fase de prueba
Agregadas las funciones nuevas en incorporando modulo gastos en fase de pruebas
</commit_message>
<xml_diff>
--- a/bd/mediclean_bd.xlsx
+++ b/bd/mediclean_bd.xlsx
@@ -623,7 +623,7 @@
       </c>
       <c r="C2" s="18" t="inlineStr">
         <is>
-          <t>kixZ-8c6in3iPLk2XvIeqPHU8gXUqV6F81iK-tZ0Oik</t>
+          <t>OefkDSQmfyFtD3meO-70Y142JJZjAmyelV6Hx6E8UBo</t>
         </is>
       </c>
     </row>
@@ -11263,7 +11263,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AN409"/>
+  <dimension ref="A1:AN410"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A192" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A192" activeCellId="0" sqref="A192"/>
@@ -28578,7 +28578,7 @@
       </c>
       <c r="K238" s="15" t="inlineStr">
         <is>
-          <t>REALIZADO</t>
+          <t>enruta</t>
         </is>
       </c>
       <c r="L238" s="15" t="inlineStr">
@@ -31075,7 +31075,7 @@
       </c>
       <c r="K275" s="15" t="inlineStr">
         <is>
-          <t>REALIZADO</t>
+          <t>enruta</t>
         </is>
       </c>
       <c r="L275" s="15" t="inlineStr">
@@ -31276,7 +31276,7 @@
       </c>
       <c r="K278" s="15" t="inlineStr">
         <is>
-          <t>REALIZADO</t>
+          <t>enruta</t>
         </is>
       </c>
       <c r="L278" s="15" t="inlineStr">
@@ -31344,7 +31344,7 @@
       </c>
       <c r="K279" s="15" t="inlineStr">
         <is>
-          <t>REALIZADO</t>
+          <t>enruta</t>
         </is>
       </c>
       <c r="L279" s="15" t="inlineStr">
@@ -31986,7 +31986,7 @@
       </c>
       <c r="K288" s="15" t="inlineStr">
         <is>
-          <t>REALIZADO</t>
+          <t>enruta</t>
         </is>
       </c>
       <c r="L288" s="15" t="inlineStr">
@@ -38102,7 +38102,7 @@
       </c>
       <c r="K378" s="15" t="inlineStr">
         <is>
-          <t>REALIZADO</t>
+          <t>enruta</t>
         </is>
       </c>
       <c r="L378" s="15" t="inlineStr">
@@ -40166,6 +40166,7 @@
         </is>
       </c>
     </row>
+    <row r="410"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -40790,10 +40791,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="15" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="K2" s="15" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L2" s="15" t="n">
         <v>7</v>
@@ -40808,7 +40809,7 @@
         <v>0</v>
       </c>
       <c r="P2" s="15" t="n">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="Q2" s="15" t="n">
         <v>0</v>

</xml_diff>